<commit_message>
More minor fixes from XLSX
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="8660" windowWidth="37660" windowHeight="13160" activeTab="1"/>
+    <workbookView xWindow="740" yWindow="8660" windowWidth="37660" windowHeight="13160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="550">
   <si>
     <t>unit</t>
   </si>
@@ -4245,8 +4245,8 @@
   <dimension ref="A1:AK452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI300" sqref="AI300"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6453,7 +6453,7 @@
         <v>2.0</v>
       </c>
       <c r="W41" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="X41" t="n">
         <v>1.0</v>
@@ -16548,7 +16548,9 @@
       <c r="B245" t="s">
         <v>39</v>
       </c>
-      <c r="C245"/>
+      <c r="C245" t="s">
+        <v>142</v>
+      </c>
       <c r="D245" t="n">
         <v>0.0</v>
       </c>

</xml_diff>

<commit_message>
Update XLSX from Dropbox
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="4875" windowWidth="37665" windowHeight="13155"/>
+    <workbookView xWindow="8670" yWindow="4875" windowWidth="37665" windowHeight="13155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2892" uniqueCount="562">
   <si>
     <t>unit</t>
   </si>
@@ -2041,16 +2041,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ34"/>
+  <dimension ref="A1:AX35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="AW2"/>
       <c r="AX2"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="AW3"/>
       <c r="AX3"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="AW4"/>
       <c r="AX4"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="AW5"/>
       <c r="AX5"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="AW8"/>
       <c r="AX8"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2782,7 +2782,7 @@
       <c r="AW9"/>
       <c r="AX9"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="AW10"/>
       <c r="AX10"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="AW11"/>
       <c r="AX11"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="AW12"/>
       <c r="AX12"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3054,7 +3054,7 @@
       <c r="AW13"/>
       <c r="AX13"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>539</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="AW14"/>
       <c r="AX14"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="AW15"/>
       <c r="AX15"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="AW16"/>
       <c r="AX16"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -3334,7 +3334,7 @@
       <c r="AW17"/>
       <c r="AX17"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -3402,7 +3402,7 @@
       <c r="AW18"/>
       <c r="AX18"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="AW19"/>
       <c r="AX19"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -3554,7 +3554,7 @@
       <c r="AW20"/>
       <c r="AX20"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -3622,7 +3622,7 @@
       <c r="AW21"/>
       <c r="AX21"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -3694,7 +3694,7 @@
       <c r="AW22"/>
       <c r="AX22"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="AW23"/>
       <c r="AX23"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="AW24"/>
       <c r="AX24"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>537</v>
       </c>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="AX25"/>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>538</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="AW27"/>
       <c r="AX27"/>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -4138,7 +4138,7 @@
       <c r="AW28"/>
       <c r="AX28"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -4210,7 +4210,7 @@
       <c r="AW29"/>
       <c r="AX29"/>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="AW30"/>
       <c r="AX30"/>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -4348,7 +4348,7 @@
       <c r="AW31"/>
       <c r="AX31"/>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -4422,7 +4422,7 @@
       <c r="AW32"/>
       <c r="AX32"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>559</v>
       </c>
@@ -4484,7 +4484,7 @@
       <c r="AW33"/>
       <c r="AX33"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="AW34"/>
       <c r="AX34"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -4637,20 +4637,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK452"/>
+  <dimension ref="A1:AL454"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D429" sqref="D429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.85546875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="AK2"/>
       <c r="AL2"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -4864,7 +4864,7 @@
       <c r="AK3"/>
       <c r="AL3"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -4914,7 +4914,7 @@
       <c r="AK4"/>
       <c r="AL4"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -4964,7 +4964,7 @@
       <c r="AK5"/>
       <c r="AL5"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -5014,7 +5014,7 @@
       <c r="AK6"/>
       <c r="AL6"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>85</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E7" t="n">
         <v>4.0</v>
@@ -5070,7 +5070,7 @@
       <c r="AK7"/>
       <c r="AL7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -5122,7 +5122,7 @@
       <c r="AK8"/>
       <c r="AL8"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -5174,7 +5174,7 @@
       <c r="AK9"/>
       <c r="AL9"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -5224,7 +5224,7 @@
       <c r="AK10"/>
       <c r="AL10"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5276,7 +5276,7 @@
       <c r="AK11"/>
       <c r="AL11"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="AK12"/>
       <c r="AL12"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -5392,7 +5392,7 @@
       <c r="AK13"/>
       <c r="AL13"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -5442,7 +5442,7 @@
       <c r="AK14"/>
       <c r="AL14"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>77</v>
       </c>
       <c r="D15" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E15" t="n">
         <v>4.0</v>
@@ -5502,7 +5502,7 @@
       <c r="AK15"/>
       <c r="AL15"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="AK16"/>
       <c r="AL16"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="AK17"/>
       <c r="AL17"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="AK18"/>
       <c r="AL18"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -5708,7 +5708,7 @@
       <c r="AK19"/>
       <c r="AL19"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>101</v>
       </c>
@@ -5766,7 +5766,7 @@
       <c r="AK20"/>
       <c r="AL20"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -5826,7 +5826,7 @@
       <c r="AK21"/>
       <c r="AL21"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="AK22"/>
       <c r="AL22"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>104</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="AK23"/>
       <c r="AL23"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -5996,7 +5996,7 @@
       <c r="AK24"/>
       <c r="AL24"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -6058,7 +6058,7 @@
       <c r="AK25"/>
       <c r="AL25"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="AK26"/>
       <c r="AL26"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -6162,7 +6162,7 @@
       <c r="AK27"/>
       <c r="AL27"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -6210,7 +6210,7 @@
       <c r="AK28"/>
       <c r="AL28"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -6264,7 +6264,7 @@
       <c r="AK29"/>
       <c r="AL29"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -6312,7 +6312,7 @@
       <c r="AK30"/>
       <c r="AL30"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -6366,7 +6366,7 @@
       <c r="AK31"/>
       <c r="AL31"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -6420,7 +6420,7 @@
       <c r="AK32"/>
       <c r="AL32"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="AK33"/>
       <c r="AL33"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -6526,7 +6526,7 @@
       <c r="AK34"/>
       <c r="AL34"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -6582,7 +6582,7 @@
       <c r="AK35"/>
       <c r="AL35"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -6636,7 +6636,7 @@
       <c r="AK36"/>
       <c r="AL36"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>120</v>
       </c>
@@ -6686,7 +6686,7 @@
       <c r="AK37"/>
       <c r="AL37"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -6744,7 +6744,7 @@
       <c r="AK38"/>
       <c r="AL38"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -6800,7 +6800,7 @@
       <c r="AK39"/>
       <c r="AL39"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>560</v>
       </c>
@@ -6846,7 +6846,7 @@
       <c r="AK40"/>
       <c r="AL40"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -6896,7 +6896,7 @@
       <c r="AK41"/>
       <c r="AL41"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -6960,7 +6960,7 @@
       <c r="AK42"/>
       <c r="AL42"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="AK43"/>
       <c r="AL43"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>126</v>
       </c>
@@ -7076,7 +7076,7 @@
       <c r="AK44"/>
       <c r="AL44"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>127</v>
       </c>
@@ -7128,7 +7128,7 @@
       <c r="AK45"/>
       <c r="AL45"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -7178,7 +7178,7 @@
       <c r="AK46"/>
       <c r="AL46"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>129</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="AK47"/>
       <c r="AL47"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -7286,7 +7286,7 @@
       <c r="AK48"/>
       <c r="AL48"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>131</v>
       </c>
@@ -7338,7 +7338,7 @@
       <c r="AK49"/>
       <c r="AL49"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>132</v>
       </c>
@@ -7390,7 +7390,7 @@
       <c r="AK50"/>
       <c r="AL50"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -7440,7 +7440,7 @@
       <c r="AK51"/>
       <c r="AL51"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>134</v>
       </c>
@@ -7492,7 +7492,7 @@
       <c r="AK52"/>
       <c r="AL52"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>135</v>
       </c>
@@ -7542,7 +7542,7 @@
       <c r="AK53"/>
       <c r="AL53"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>136</v>
       </c>
@@ -7592,7 +7592,7 @@
       <c r="AK54"/>
       <c r="AL54"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>137</v>
       </c>
@@ -7640,7 +7640,7 @@
       <c r="AK55"/>
       <c r="AL55"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>138</v>
       </c>
@@ -7688,7 +7688,7 @@
       <c r="AK56"/>
       <c r="AL56"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>139</v>
       </c>
@@ -7738,7 +7738,7 @@
       <c r="AK57"/>
       <c r="AL57"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>141</v>
       </c>
@@ -7790,7 +7790,7 @@
       <c r="AK58"/>
       <c r="AL58"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -7836,7 +7836,7 @@
       <c r="AK59"/>
       <c r="AL59"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -7896,7 +7896,7 @@
       <c r="AK60"/>
       <c r="AL60"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>144</v>
       </c>
@@ -7946,7 +7946,7 @@
       <c r="AK61"/>
       <c r="AL61"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>145</v>
       </c>
@@ -7996,7 +7996,7 @@
       <c r="AK62"/>
       <c r="AL62"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -8054,7 +8054,7 @@
       <c r="AK63"/>
       <c r="AL63"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>147</v>
       </c>
@@ -8104,7 +8104,7 @@
       <c r="AK64"/>
       <c r="AL64"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -8158,7 +8158,7 @@
       <c r="AK65"/>
       <c r="AL65"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>81</v>
       </c>
       <c r="D66" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E66" t="n">
         <v>2.0</v>
@@ -8214,7 +8214,7 @@
       <c r="AK66"/>
       <c r="AL66"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -8264,7 +8264,7 @@
       <c r="AK67"/>
       <c r="AL67"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>151</v>
       </c>
@@ -8314,7 +8314,7 @@
       <c r="AK68"/>
       <c r="AL68"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>152</v>
       </c>
@@ -8364,7 +8364,7 @@
       <c r="AK69"/>
       <c r="AL69"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -8414,7 +8414,7 @@
       <c r="AK70"/>
       <c r="AL70"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>154</v>
       </c>
@@ -8474,7 +8474,7 @@
       <c r="AK71"/>
       <c r="AL71"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>155</v>
       </c>
@@ -8530,7 +8530,7 @@
       <c r="AK72"/>
       <c r="AL72"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>156</v>
       </c>
@@ -8594,7 +8594,7 @@
       <c r="AK73"/>
       <c r="AL73"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>157</v>
       </c>
@@ -8644,7 +8644,7 @@
       <c r="AK74"/>
       <c r="AL74"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>158</v>
       </c>
@@ -8694,7 +8694,7 @@
       <c r="AK75"/>
       <c r="AL75"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -8744,7 +8744,7 @@
       <c r="AK76"/>
       <c r="AL76"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>160</v>
       </c>
@@ -8802,7 +8802,7 @@
       <c r="AK77"/>
       <c r="AL77"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -8858,7 +8858,7 @@
       <c r="AK78"/>
       <c r="AL78"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="AK79"/>
       <c r="AL79"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -8960,7 +8960,7 @@
       <c r="AK80"/>
       <c r="AL80"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -9006,7 +9006,7 @@
       <c r="AK81"/>
       <c r="AL81"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -9060,7 +9060,7 @@
       <c r="AK82"/>
       <c r="AL82"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>166</v>
       </c>
@@ -9110,7 +9110,7 @@
       <c r="AK83"/>
       <c r="AL83"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>167</v>
       </c>
@@ -9160,7 +9160,7 @@
       <c r="AK84"/>
       <c r="AL84"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>168</v>
       </c>
@@ -9214,7 +9214,7 @@
       <c r="AK85"/>
       <c r="AL85"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>169</v>
       </c>
@@ -9272,7 +9272,7 @@
       <c r="AK86"/>
       <c r="AL86"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -9322,7 +9322,7 @@
       <c r="AK87"/>
       <c r="AL87"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -9388,7 +9388,7 @@
       <c r="AK88"/>
       <c r="AL88"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>172</v>
       </c>
@@ -9436,7 +9436,7 @@
       <c r="AK89"/>
       <c r="AL89"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>173</v>
       </c>
@@ -9488,7 +9488,7 @@
       <c r="AK90"/>
       <c r="AL90"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>174</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="AK91"/>
       <c r="AL91"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -9590,7 +9590,7 @@
       <c r="AK92"/>
       <c r="AL92"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>176</v>
       </c>
@@ -9646,7 +9646,7 @@
       <c r="AK93"/>
       <c r="AL93"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>177</v>
       </c>
@@ -9698,7 +9698,7 @@
       <c r="AK94"/>
       <c r="AL94"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -9748,7 +9748,7 @@
       <c r="AK95"/>
       <c r="AL95"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>179</v>
       </c>
@@ -9800,7 +9800,7 @@
       <c r="AK96"/>
       <c r="AL96"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>180</v>
       </c>
@@ -9852,7 +9852,7 @@
       <c r="AK97"/>
       <c r="AL97"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -9914,7 +9914,7 @@
       <c r="AK98"/>
       <c r="AL98"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>182</v>
       </c>
@@ -9972,7 +9972,7 @@
       <c r="AK99"/>
       <c r="AL99"/>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -10022,7 +10022,7 @@
       <c r="AK100"/>
       <c r="AL100"/>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -10078,7 +10078,7 @@
       <c r="AK101"/>
       <c r="AL101"/>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>185</v>
       </c>
@@ -10130,7 +10130,7 @@
       <c r="AK102"/>
       <c r="AL102"/>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>186</v>
       </c>
@@ -10196,7 +10196,7 @@
       <c r="AK103"/>
       <c r="AL103"/>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>187</v>
       </c>
@@ -10252,7 +10252,7 @@
       <c r="AK104"/>
       <c r="AL104"/>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>188</v>
       </c>
@@ -10312,7 +10312,7 @@
       <c r="AK105"/>
       <c r="AL105"/>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>189</v>
       </c>
@@ -10366,7 +10366,7 @@
       <c r="AK106"/>
       <c r="AL106"/>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>190</v>
       </c>
@@ -10416,7 +10416,7 @@
       <c r="AK107"/>
       <c r="AL107"/>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>191</v>
       </c>
@@ -10478,7 +10478,7 @@
       <c r="AK108"/>
       <c r="AL108"/>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>192</v>
       </c>
@@ -10530,7 +10530,7 @@
       <c r="AK109"/>
       <c r="AL109"/>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>193</v>
       </c>
@@ -10582,7 +10582,7 @@
       <c r="AK110"/>
       <c r="AL110"/>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>194</v>
       </c>
@@ -10640,7 +10640,7 @@
       <c r="AK111"/>
       <c r="AL111"/>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>195</v>
       </c>
@@ -10696,7 +10696,7 @@
       <c r="AK112"/>
       <c r="AL112"/>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>196</v>
       </c>
@@ -10754,7 +10754,7 @@
       <c r="AK113"/>
       <c r="AL113"/>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>197</v>
       </c>
@@ -10816,7 +10816,7 @@
       <c r="AK114"/>
       <c r="AL114"/>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>198</v>
       </c>
@@ -10866,7 +10866,7 @@
       <c r="AK115"/>
       <c r="AL115"/>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>199</v>
       </c>
@@ -10916,7 +10916,7 @@
       <c r="AK116"/>
       <c r="AL116"/>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>200</v>
       </c>
@@ -10972,7 +10972,7 @@
       <c r="AK117"/>
       <c r="AL117"/>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>201</v>
       </c>
@@ -11030,7 +11030,7 @@
       <c r="AK118"/>
       <c r="AL118"/>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>202</v>
       </c>
@@ -11086,7 +11086,7 @@
       <c r="AK119"/>
       <c r="AL119"/>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>203</v>
       </c>
@@ -11136,7 +11136,7 @@
       <c r="AK120"/>
       <c r="AL120"/>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>204</v>
       </c>
@@ -11190,7 +11190,7 @@
       <c r="AK121"/>
       <c r="AL121"/>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>205</v>
       </c>
@@ -11242,7 +11242,7 @@
       <c r="AK122"/>
       <c r="AL122"/>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>206</v>
       </c>
@@ -11292,7 +11292,7 @@
       <c r="AK123"/>
       <c r="AL123"/>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>207</v>
       </c>
@@ -11346,7 +11346,7 @@
       <c r="AK124"/>
       <c r="AL124"/>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>208</v>
       </c>
@@ -11398,7 +11398,7 @@
       <c r="AK125"/>
       <c r="AL125"/>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>209</v>
       </c>
@@ -11444,7 +11444,7 @@
       <c r="AK126"/>
       <c r="AL126"/>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>210</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="AK127"/>
       <c r="AL127"/>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>211</v>
       </c>
@@ -11546,7 +11546,7 @@
       <c r="AK128"/>
       <c r="AL128"/>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>212</v>
       </c>
@@ -11598,7 +11598,7 @@
       <c r="AK129"/>
       <c r="AL129"/>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>561</v>
       </c>
@@ -11628,7 +11628,7 @@
       <c r="U130"/>
       <c r="V130"/>
       <c r="W130" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="X130"/>
       <c r="Y130"/>
@@ -11646,7 +11646,7 @@
       <c r="AK130"/>
       <c r="AL130"/>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>213</v>
       </c>
@@ -11708,7 +11708,7 @@
       <c r="AK131"/>
       <c r="AL131"/>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>214</v>
       </c>
@@ -11768,7 +11768,7 @@
       <c r="AK132"/>
       <c r="AL132"/>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>215</v>
       </c>
@@ -11820,7 +11820,7 @@
       <c r="AK133"/>
       <c r="AL133"/>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>216</v>
       </c>
@@ -11866,7 +11866,7 @@
       <c r="AK134"/>
       <c r="AL134"/>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>217</v>
       </c>
@@ -11916,7 +11916,7 @@
       <c r="AK135"/>
       <c r="AL135"/>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>218</v>
       </c>
@@ -11978,7 +11978,7 @@
       <c r="AK136"/>
       <c r="AL136"/>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>219</v>
       </c>
@@ -12032,7 +12032,7 @@
       <c r="AK137"/>
       <c r="AL137"/>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>220</v>
       </c>
@@ -12092,7 +12092,7 @@
       <c r="AK138"/>
       <c r="AL138"/>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>221</v>
       </c>
@@ -12144,7 +12144,7 @@
       <c r="AK139"/>
       <c r="AL139"/>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -12194,7 +12194,7 @@
       <c r="AK140"/>
       <c r="AL140"/>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>223</v>
       </c>
@@ -12244,7 +12244,7 @@
       <c r="AK141"/>
       <c r="AL141"/>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>224</v>
       </c>
@@ -12304,7 +12304,7 @@
       <c r="AK142"/>
       <c r="AL142"/>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>225</v>
       </c>
@@ -12362,7 +12362,7 @@
       <c r="AK143"/>
       <c r="AL143"/>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>226</v>
       </c>
@@ -12414,7 +12414,7 @@
       <c r="AK144"/>
       <c r="AL144"/>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>227</v>
       </c>
@@ -12468,7 +12468,7 @@
       <c r="AK145"/>
       <c r="AL145"/>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>228</v>
       </c>
@@ -12520,7 +12520,7 @@
       <c r="AK146"/>
       <c r="AL146"/>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>229</v>
       </c>
@@ -12568,7 +12568,7 @@
       <c r="AK147"/>
       <c r="AL147"/>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>230</v>
       </c>
@@ -12628,7 +12628,7 @@
       <c r="AK148"/>
       <c r="AL148"/>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>231</v>
       </c>
@@ -12692,7 +12692,7 @@
       <c r="AK149"/>
       <c r="AL149"/>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>232</v>
       </c>
@@ -12744,7 +12744,7 @@
       <c r="AK150"/>
       <c r="AL150"/>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>233</v>
       </c>
@@ -12794,7 +12794,7 @@
       <c r="AK151"/>
       <c r="AL151"/>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>234</v>
       </c>
@@ -12846,7 +12846,7 @@
       <c r="AK152"/>
       <c r="AL152"/>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>235</v>
       </c>
@@ -12892,7 +12892,7 @@
       <c r="AK153"/>
       <c r="AL153"/>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>236</v>
       </c>
@@ -12938,7 +12938,7 @@
       <c r="AK154"/>
       <c r="AL154"/>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>237</v>
       </c>
@@ -12984,7 +12984,7 @@
       <c r="AK155"/>
       <c r="AL155"/>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>238</v>
       </c>
@@ -13030,7 +13030,7 @@
       <c r="AK156"/>
       <c r="AL156"/>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>239</v>
       </c>
@@ -13076,7 +13076,7 @@
       <c r="AK157"/>
       <c r="AL157"/>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>240</v>
       </c>
@@ -13122,7 +13122,7 @@
       <c r="AK158"/>
       <c r="AL158"/>
     </row>
-    <row r="159" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>241</v>
       </c>
@@ -13168,7 +13168,7 @@
       <c r="AK159"/>
       <c r="AL159"/>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>242</v>
       </c>
@@ -13214,7 +13214,7 @@
       <c r="AK160"/>
       <c r="AL160"/>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>243</v>
       </c>
@@ -13266,7 +13266,7 @@
       <c r="AK161"/>
       <c r="AL161"/>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>244</v>
       </c>
@@ -13318,7 +13318,7 @@
       <c r="AK162"/>
       <c r="AL162"/>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>245</v>
       </c>
@@ -13364,7 +13364,7 @@
       <c r="AK163"/>
       <c r="AL163"/>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>246</v>
       </c>
@@ -13410,7 +13410,7 @@
       <c r="AK164"/>
       <c r="AL164"/>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>247</v>
       </c>
@@ -13456,7 +13456,7 @@
       <c r="AK165"/>
       <c r="AL165"/>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>248</v>
       </c>
@@ -13502,7 +13502,7 @@
       <c r="AK166"/>
       <c r="AL166"/>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>249</v>
       </c>
@@ -13548,7 +13548,7 @@
       <c r="AK167"/>
       <c r="AL167"/>
     </row>
-    <row r="168" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>250</v>
       </c>
@@ -13594,7 +13594,7 @@
       <c r="AK168"/>
       <c r="AL168"/>
     </row>
-    <row r="169" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>251</v>
       </c>
@@ -13640,7 +13640,7 @@
       <c r="AK169"/>
       <c r="AL169"/>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>252</v>
       </c>
@@ -13692,7 +13692,7 @@
       <c r="AK170"/>
       <c r="AL170"/>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>253</v>
       </c>
@@ -13738,7 +13738,7 @@
       <c r="AK171"/>
       <c r="AL171"/>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>254</v>
       </c>
@@ -13790,7 +13790,7 @@
       <c r="AK172"/>
       <c r="AL172"/>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>255</v>
       </c>
@@ -13842,7 +13842,7 @@
       <c r="AK173"/>
       <c r="AL173"/>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>256</v>
       </c>
@@ -13894,7 +13894,7 @@
       <c r="AK174"/>
       <c r="AL174"/>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>257</v>
       </c>
@@ -13940,7 +13940,7 @@
       <c r="AK175"/>
       <c r="AL175"/>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>258</v>
       </c>
@@ -13986,7 +13986,7 @@
       <c r="AK176"/>
       <c r="AL176"/>
     </row>
-    <row r="177" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>259</v>
       </c>
@@ -14038,7 +14038,7 @@
       <c r="AK177"/>
       <c r="AL177"/>
     </row>
-    <row r="178" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>260</v>
       </c>
@@ -14084,7 +14084,7 @@
       <c r="AK178"/>
       <c r="AL178"/>
     </row>
-    <row r="179" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>261</v>
       </c>
@@ -14130,7 +14130,7 @@
       <c r="AK179"/>
       <c r="AL179"/>
     </row>
-    <row r="180" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>262</v>
       </c>
@@ -14176,7 +14176,7 @@
       <c r="AK180"/>
       <c r="AL180"/>
     </row>
-    <row r="181" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>263</v>
       </c>
@@ -14222,7 +14222,7 @@
       <c r="AK181"/>
       <c r="AL181"/>
     </row>
-    <row r="182" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>264</v>
       </c>
@@ -14268,7 +14268,7 @@
       <c r="AK182"/>
       <c r="AL182"/>
     </row>
-    <row r="183" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>265</v>
       </c>
@@ -14314,7 +14314,7 @@
       <c r="AK183"/>
       <c r="AL183"/>
     </row>
-    <row r="184" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>266</v>
       </c>
@@ -14360,7 +14360,7 @@
       <c r="AK184"/>
       <c r="AL184"/>
     </row>
-    <row r="185" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>267</v>
       </c>
@@ -14406,7 +14406,7 @@
       <c r="AK185"/>
       <c r="AL185"/>
     </row>
-    <row r="186" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>268</v>
       </c>
@@ -14456,7 +14456,7 @@
       <c r="AK186"/>
       <c r="AL186"/>
     </row>
-    <row r="187" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>269</v>
       </c>
@@ -14502,7 +14502,7 @@
       <c r="AK187"/>
       <c r="AL187"/>
     </row>
-    <row r="188" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>270</v>
       </c>
@@ -14548,7 +14548,7 @@
       <c r="AK188"/>
       <c r="AL188"/>
     </row>
-    <row r="189" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>271</v>
       </c>
@@ -14594,7 +14594,7 @@
       <c r="AK189"/>
       <c r="AL189"/>
     </row>
-    <row r="190" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>272</v>
       </c>
@@ -14646,7 +14646,7 @@
       <c r="AK190"/>
       <c r="AL190"/>
     </row>
-    <row r="191" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>273</v>
       </c>
@@ -14698,7 +14698,7 @@
       <c r="AK191"/>
       <c r="AL191"/>
     </row>
-    <row r="192" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>274</v>
       </c>
@@ -14744,7 +14744,7 @@
       <c r="AK192"/>
       <c r="AL192"/>
     </row>
-    <row r="193" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>275</v>
       </c>
@@ -14790,7 +14790,7 @@
       <c r="AK193"/>
       <c r="AL193"/>
     </row>
-    <row r="194" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>276</v>
       </c>
@@ -14836,7 +14836,7 @@
       <c r="AK194"/>
       <c r="AL194"/>
     </row>
-    <row r="195" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>277</v>
       </c>
@@ -14882,7 +14882,7 @@
       <c r="AK195"/>
       <c r="AL195"/>
     </row>
-    <row r="196" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>278</v>
       </c>
@@ -14934,7 +14934,7 @@
       <c r="AK196"/>
       <c r="AL196"/>
     </row>
-    <row r="197" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>279</v>
       </c>
@@ -14986,7 +14986,7 @@
       <c r="AK197"/>
       <c r="AL197"/>
     </row>
-    <row r="198" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>280</v>
       </c>
@@ -15032,7 +15032,7 @@
       <c r="AK198"/>
       <c r="AL198"/>
     </row>
-    <row r="199" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>281</v>
       </c>
@@ -15040,7 +15040,9 @@
         <v>37</v>
       </c>
       <c r="C199"/>
-      <c r="D199"/>
+      <c r="D199" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E199"/>
       <c r="F199"/>
       <c r="G199"/>
@@ -15076,7 +15078,7 @@
       <c r="AK199"/>
       <c r="AL199"/>
     </row>
-    <row r="200" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>282</v>
       </c>
@@ -15084,7 +15086,9 @@
         <v>37</v>
       </c>
       <c r="C200"/>
-      <c r="D200"/>
+      <c r="D200" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E200"/>
       <c r="F200"/>
       <c r="G200"/>
@@ -15120,7 +15124,7 @@
       <c r="AK200"/>
       <c r="AL200"/>
     </row>
-    <row r="201" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>283</v>
       </c>
@@ -15128,7 +15132,9 @@
         <v>37</v>
       </c>
       <c r="C201"/>
-      <c r="D201"/>
+      <c r="D201" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E201"/>
       <c r="F201"/>
       <c r="G201"/>
@@ -15164,7 +15170,7 @@
       <c r="AK201"/>
       <c r="AL201"/>
     </row>
-    <row r="202" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>284</v>
       </c>
@@ -15172,7 +15178,9 @@
         <v>37</v>
       </c>
       <c r="C202"/>
-      <c r="D202"/>
+      <c r="D202" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E202"/>
       <c r="F202"/>
       <c r="G202"/>
@@ -15208,7 +15216,7 @@
       <c r="AK202"/>
       <c r="AL202"/>
     </row>
-    <row r="203" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>285</v>
       </c>
@@ -15216,7 +15224,9 @@
         <v>37</v>
       </c>
       <c r="C203"/>
-      <c r="D203"/>
+      <c r="D203" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E203"/>
       <c r="F203"/>
       <c r="G203"/>
@@ -15252,7 +15262,7 @@
       <c r="AK203"/>
       <c r="AL203"/>
     </row>
-    <row r="204" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>286</v>
       </c>
@@ -15260,7 +15270,9 @@
         <v>37</v>
       </c>
       <c r="C204"/>
-      <c r="D204"/>
+      <c r="D204" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E204"/>
       <c r="F204"/>
       <c r="G204"/>
@@ -15296,7 +15308,7 @@
       <c r="AK204"/>
       <c r="AL204"/>
     </row>
-    <row r="205" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>287</v>
       </c>
@@ -15304,7 +15316,9 @@
         <v>37</v>
       </c>
       <c r="C205"/>
-      <c r="D205"/>
+      <c r="D205" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E205"/>
       <c r="F205"/>
       <c r="G205"/>
@@ -15340,7 +15354,7 @@
       <c r="AK205"/>
       <c r="AL205"/>
     </row>
-    <row r="206" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>288</v>
       </c>
@@ -15348,7 +15362,9 @@
         <v>37</v>
       </c>
       <c r="C206"/>
-      <c r="D206"/>
+      <c r="D206" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E206"/>
       <c r="F206"/>
       <c r="G206"/>
@@ -15384,7 +15400,7 @@
       <c r="AK206"/>
       <c r="AL206"/>
     </row>
-    <row r="207" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>289</v>
       </c>
@@ -15430,7 +15446,7 @@
       <c r="AK207"/>
       <c r="AL207"/>
     </row>
-    <row r="208" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>290</v>
       </c>
@@ -15476,7 +15492,7 @@
       <c r="AK208"/>
       <c r="AL208"/>
     </row>
-    <row r="209" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>291</v>
       </c>
@@ -15528,7 +15544,7 @@
       <c r="AK209"/>
       <c r="AL209"/>
     </row>
-    <row r="210" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>292</v>
       </c>
@@ -15578,7 +15594,7 @@
       <c r="AK210"/>
       <c r="AL210"/>
     </row>
-    <row r="211" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>293</v>
       </c>
@@ -15624,7 +15640,7 @@
       <c r="AK211"/>
       <c r="AL211"/>
     </row>
-    <row r="212" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>294</v>
       </c>
@@ -15670,7 +15686,7 @@
       <c r="AK212"/>
       <c r="AL212"/>
     </row>
-    <row r="213" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>295</v>
       </c>
@@ -15722,7 +15738,7 @@
       <c r="AK213"/>
       <c r="AL213"/>
     </row>
-    <row r="214" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>296</v>
       </c>
@@ -15774,7 +15790,7 @@
       <c r="AK214"/>
       <c r="AL214"/>
     </row>
-    <row r="215" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>297</v>
       </c>
@@ -15820,7 +15836,7 @@
       <c r="AK215"/>
       <c r="AL215"/>
     </row>
-    <row r="216" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>298</v>
       </c>
@@ -15866,7 +15882,7 @@
       <c r="AK216"/>
       <c r="AL216"/>
     </row>
-    <row r="217" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>299</v>
       </c>
@@ -15918,7 +15934,7 @@
       <c r="AK217"/>
       <c r="AL217"/>
     </row>
-    <row r="218" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>300</v>
       </c>
@@ -15964,7 +15980,7 @@
       <c r="AK218"/>
       <c r="AL218"/>
     </row>
-    <row r="219" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>301</v>
       </c>
@@ -16010,7 +16026,7 @@
       <c r="AK219"/>
       <c r="AL219"/>
     </row>
-    <row r="220" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>302</v>
       </c>
@@ -16060,7 +16076,7 @@
       <c r="AK220"/>
       <c r="AL220"/>
     </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>303</v>
       </c>
@@ -16106,7 +16122,7 @@
       <c r="AK221"/>
       <c r="AL221"/>
     </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>304</v>
       </c>
@@ -16156,7 +16172,7 @@
       <c r="AK222"/>
       <c r="AL222"/>
     </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>305</v>
       </c>
@@ -16202,7 +16218,7 @@
       <c r="AK223"/>
       <c r="AL223"/>
     </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>306</v>
       </c>
@@ -16248,7 +16264,7 @@
       <c r="AK224"/>
       <c r="AL224"/>
     </row>
-    <row r="225" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>307</v>
       </c>
@@ -16294,7 +16310,7 @@
       <c r="AK225"/>
       <c r="AL225"/>
     </row>
-    <row r="226" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>308</v>
       </c>
@@ -16340,7 +16356,7 @@
       <c r="AK226"/>
       <c r="AL226"/>
     </row>
-    <row r="227" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>309</v>
       </c>
@@ -16386,7 +16402,7 @@
       <c r="AK227"/>
       <c r="AL227"/>
     </row>
-    <row r="228" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>310</v>
       </c>
@@ -16432,7 +16448,7 @@
       <c r="AK228"/>
       <c r="AL228"/>
     </row>
-    <row r="229" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>311</v>
       </c>
@@ -16478,7 +16494,7 @@
       <c r="AK229"/>
       <c r="AL229"/>
     </row>
-    <row r="230" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>312</v>
       </c>
@@ -16524,7 +16540,7 @@
       <c r="AK230"/>
       <c r="AL230"/>
     </row>
-    <row r="231" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>313</v>
       </c>
@@ -16576,7 +16592,7 @@
       <c r="AK231"/>
       <c r="AL231"/>
     </row>
-    <row r="232" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>314</v>
       </c>
@@ -16622,7 +16638,7 @@
       <c r="AK232"/>
       <c r="AL232"/>
     </row>
-    <row r="233" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>315</v>
       </c>
@@ -16668,7 +16684,7 @@
       <c r="AK233"/>
       <c r="AL233"/>
     </row>
-    <row r="234" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>316</v>
       </c>
@@ -16718,7 +16734,7 @@
       <c r="AK234"/>
       <c r="AL234"/>
     </row>
-    <row r="235" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>317</v>
       </c>
@@ -16770,7 +16786,7 @@
       <c r="AK235"/>
       <c r="AL235"/>
     </row>
-    <row r="236" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>318</v>
       </c>
@@ -16816,7 +16832,7 @@
       <c r="AK236"/>
       <c r="AL236"/>
     </row>
-    <row r="237" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>319</v>
       </c>
@@ -16862,7 +16878,7 @@
       <c r="AK237"/>
       <c r="AL237"/>
     </row>
-    <row r="238" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>320</v>
       </c>
@@ -16914,7 +16930,7 @@
       <c r="AK238"/>
       <c r="AL238"/>
     </row>
-    <row r="239" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>321</v>
       </c>
@@ -16960,7 +16976,7 @@
       <c r="AK239"/>
       <c r="AL239"/>
     </row>
-    <row r="240" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>322</v>
       </c>
@@ -17006,7 +17022,7 @@
       <c r="AK240"/>
       <c r="AL240"/>
     </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>323</v>
       </c>
@@ -17052,7 +17068,7 @@
       <c r="AK241"/>
       <c r="AL241"/>
     </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>324</v>
       </c>
@@ -17098,7 +17114,7 @@
       <c r="AK242"/>
       <c r="AL242"/>
     </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>325</v>
       </c>
@@ -17150,7 +17166,7 @@
       <c r="AK243"/>
       <c r="AL243"/>
     </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>326</v>
       </c>
@@ -17196,7 +17212,7 @@
       <c r="AK244"/>
       <c r="AL244"/>
     </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>327</v>
       </c>
@@ -17242,7 +17258,7 @@
       <c r="AK245"/>
       <c r="AL245"/>
     </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>328</v>
       </c>
@@ -17288,7 +17304,7 @@
       <c r="AK246"/>
       <c r="AL246"/>
     </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>329</v>
       </c>
@@ -17340,7 +17356,7 @@
       <c r="AK247"/>
       <c r="AL247"/>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>330</v>
       </c>
@@ -17386,7 +17402,7 @@
       <c r="AK248"/>
       <c r="AL248"/>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>331</v>
       </c>
@@ -17432,7 +17448,7 @@
       <c r="AK249"/>
       <c r="AL249"/>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>332</v>
       </c>
@@ -17478,7 +17494,7 @@
       <c r="AK250"/>
       <c r="AL250"/>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>333</v>
       </c>
@@ -17524,7 +17540,7 @@
       <c r="AK251"/>
       <c r="AL251"/>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>334</v>
       </c>
@@ -17576,7 +17592,7 @@
       <c r="AK252"/>
       <c r="AL252"/>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>335</v>
       </c>
@@ -17622,7 +17638,7 @@
       <c r="AK253"/>
       <c r="AL253"/>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>336</v>
       </c>
@@ -17668,7 +17684,7 @@
       <c r="AK254"/>
       <c r="AL254"/>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>337</v>
       </c>
@@ -17720,7 +17736,7 @@
       <c r="AK255"/>
       <c r="AL255"/>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>338</v>
       </c>
@@ -17766,7 +17782,7 @@
       <c r="AK256"/>
       <c r="AL256"/>
     </row>
-    <row r="257" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>339</v>
       </c>
@@ -17812,7 +17828,7 @@
       <c r="AK257"/>
       <c r="AL257"/>
     </row>
-    <row r="258" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>340</v>
       </c>
@@ -17862,7 +17878,7 @@
       <c r="AK258"/>
       <c r="AL258"/>
     </row>
-    <row r="259" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>341</v>
       </c>
@@ -17908,7 +17924,7 @@
       <c r="AK259"/>
       <c r="AL259"/>
     </row>
-    <row r="260" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>342</v>
       </c>
@@ -17954,7 +17970,7 @@
       <c r="AK260"/>
       <c r="AL260"/>
     </row>
-    <row r="261" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>343</v>
       </c>
@@ -18000,7 +18016,7 @@
       <c r="AK261"/>
       <c r="AL261"/>
     </row>
-    <row r="262" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>344</v>
       </c>
@@ -18046,7 +18062,7 @@
       <c r="AK262"/>
       <c r="AL262"/>
     </row>
-    <row r="263" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>345</v>
       </c>
@@ -18096,7 +18112,7 @@
       <c r="AK263"/>
       <c r="AL263"/>
     </row>
-    <row r="264" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>346</v>
       </c>
@@ -18142,7 +18158,7 @@
       <c r="AK264"/>
       <c r="AL264"/>
     </row>
-    <row r="265" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>347</v>
       </c>
@@ -18188,7 +18204,7 @@
       <c r="AK265"/>
       <c r="AL265"/>
     </row>
-    <row r="266" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>348</v>
       </c>
@@ -18240,7 +18256,7 @@
       <c r="AK266"/>
       <c r="AL266"/>
     </row>
-    <row r="267" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>349</v>
       </c>
@@ -18286,7 +18302,7 @@
       <c r="AK267"/>
       <c r="AL267"/>
     </row>
-    <row r="268" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>350</v>
       </c>
@@ -18332,7 +18348,7 @@
       <c r="AK268"/>
       <c r="AL268"/>
     </row>
-    <row r="269" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>351</v>
       </c>
@@ -18378,7 +18394,7 @@
       <c r="AK269"/>
       <c r="AL269"/>
     </row>
-    <row r="270" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>352</v>
       </c>
@@ -18424,7 +18440,7 @@
       <c r="AK270"/>
       <c r="AL270"/>
     </row>
-    <row r="271" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>353</v>
       </c>
@@ -18474,7 +18490,7 @@
       <c r="AK271"/>
       <c r="AL271"/>
     </row>
-    <row r="272" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>354</v>
       </c>
@@ -18520,7 +18536,7 @@
       <c r="AK272"/>
       <c r="AL272"/>
     </row>
-    <row r="273" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>355</v>
       </c>
@@ -18566,7 +18582,7 @@
       <c r="AK273"/>
       <c r="AL273"/>
     </row>
-    <row r="274" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>356</v>
       </c>
@@ -18612,7 +18628,7 @@
       <c r="AK274"/>
       <c r="AL274"/>
     </row>
-    <row r="275" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>357</v>
       </c>
@@ -18658,7 +18674,7 @@
       <c r="AK275"/>
       <c r="AL275"/>
     </row>
-    <row r="276" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>358</v>
       </c>
@@ -18704,7 +18720,7 @@
       <c r="AK276"/>
       <c r="AL276"/>
     </row>
-    <row r="277" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>359</v>
       </c>
@@ -18750,7 +18766,7 @@
       <c r="AK277"/>
       <c r="AL277"/>
     </row>
-    <row r="278" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>360</v>
       </c>
@@ -18796,7 +18812,7 @@
       <c r="AK278"/>
       <c r="AL278"/>
     </row>
-    <row r="279" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>361</v>
       </c>
@@ -18842,7 +18858,7 @@
       <c r="AK279"/>
       <c r="AL279"/>
     </row>
-    <row r="280" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>362</v>
       </c>
@@ -18888,7 +18904,7 @@
       <c r="AK280"/>
       <c r="AL280"/>
     </row>
-    <row r="281" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>363</v>
       </c>
@@ -18940,7 +18956,7 @@
       <c r="AK281"/>
       <c r="AL281"/>
     </row>
-    <row r="282" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>364</v>
       </c>
@@ -18986,7 +19002,7 @@
       <c r="AK282"/>
       <c r="AL282"/>
     </row>
-    <row r="283" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>365</v>
       </c>
@@ -19032,7 +19048,7 @@
       <c r="AK283"/>
       <c r="AL283"/>
     </row>
-    <row r="284" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>366</v>
       </c>
@@ -19082,7 +19098,7 @@
       <c r="AK284"/>
       <c r="AL284"/>
     </row>
-    <row r="285" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>367</v>
       </c>
@@ -19128,7 +19144,7 @@
       <c r="AK285"/>
       <c r="AL285"/>
     </row>
-    <row r="286" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>368</v>
       </c>
@@ -19180,7 +19196,7 @@
       <c r="AK286"/>
       <c r="AL286"/>
     </row>
-    <row r="287" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>369</v>
       </c>
@@ -19226,7 +19242,7 @@
       <c r="AK287"/>
       <c r="AL287"/>
     </row>
-    <row r="288" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>370</v>
       </c>
@@ -19272,7 +19288,7 @@
       <c r="AK288"/>
       <c r="AL288"/>
     </row>
-    <row r="289" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>371</v>
       </c>
@@ -19318,7 +19334,7 @@
       <c r="AK289"/>
       <c r="AL289"/>
     </row>
-    <row r="290" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>372</v>
       </c>
@@ -19364,7 +19380,7 @@
       <c r="AK290"/>
       <c r="AL290"/>
     </row>
-    <row r="291" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>373</v>
       </c>
@@ -19410,7 +19426,7 @@
       <c r="AK291"/>
       <c r="AL291"/>
     </row>
-    <row r="292" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>374</v>
       </c>
@@ -19456,7 +19472,7 @@
       <c r="AK292"/>
       <c r="AL292"/>
     </row>
-    <row r="293" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>375</v>
       </c>
@@ -19502,7 +19518,7 @@
       <c r="AK293"/>
       <c r="AL293"/>
     </row>
-    <row r="294" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>376</v>
       </c>
@@ -19548,7 +19564,7 @@
       <c r="AK294"/>
       <c r="AL294"/>
     </row>
-    <row r="295" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>377</v>
       </c>
@@ -19594,7 +19610,7 @@
       <c r="AK295"/>
       <c r="AL295"/>
     </row>
-    <row r="296" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>378</v>
       </c>
@@ -19640,7 +19656,7 @@
       <c r="AK296"/>
       <c r="AL296"/>
     </row>
-    <row r="297" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>379</v>
       </c>
@@ -19686,7 +19702,7 @@
       <c r="AK297"/>
       <c r="AL297"/>
     </row>
-    <row r="298" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>380</v>
       </c>
@@ -19732,7 +19748,7 @@
       <c r="AK298"/>
       <c r="AL298"/>
     </row>
-    <row r="299" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>381</v>
       </c>
@@ -19778,7 +19794,7 @@
       <c r="AK299"/>
       <c r="AL299"/>
     </row>
-    <row r="300" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>382</v>
       </c>
@@ -19832,7 +19848,7 @@
       <c r="AK300"/>
       <c r="AL300"/>
     </row>
-    <row r="301" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>383</v>
       </c>
@@ -19886,7 +19902,7 @@
       <c r="AK301"/>
       <c r="AL301"/>
     </row>
-    <row r="302" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>384</v>
       </c>
@@ -19897,7 +19913,7 @@
         <v>77</v>
       </c>
       <c r="D302" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="E302" t="n">
         <v>3.0</v>
@@ -19946,7 +19962,7 @@
       <c r="AK302"/>
       <c r="AL302"/>
     </row>
-    <row r="303" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>385</v>
       </c>
@@ -19996,7 +20012,7 @@
       <c r="AK303"/>
       <c r="AL303"/>
     </row>
-    <row r="304" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>386</v>
       </c>
@@ -20321,7 +20337,7 @@
         <v>81</v>
       </c>
       <c r="D310" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E310" t="n">
         <v>3.0</v>
@@ -20489,7 +20505,7 @@
         <v>77</v>
       </c>
       <c r="D313" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E313" t="n">
         <v>2.0</v>
@@ -20902,7 +20918,7 @@
       <c r="AK320"/>
       <c r="AL320"/>
     </row>
-    <row r="321" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>403</v>
       </c>
@@ -20962,7 +20978,7 @@
       <c r="AK321"/>
       <c r="AL321"/>
     </row>
-    <row r="322" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>404</v>
       </c>
@@ -21008,7 +21024,7 @@
       <c r="AK322"/>
       <c r="AL322"/>
     </row>
-    <row r="323" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>405</v>
       </c>
@@ -21054,7 +21070,7 @@
       <c r="AK323"/>
       <c r="AL323"/>
     </row>
-    <row r="324" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>406</v>
       </c>
@@ -21116,7 +21132,7 @@
       <c r="AK324"/>
       <c r="AL324"/>
     </row>
-    <row r="325" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>407</v>
       </c>
@@ -21172,7 +21188,7 @@
       <c r="AK325"/>
       <c r="AL325"/>
     </row>
-    <row r="326" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>408</v>
       </c>
@@ -21234,7 +21250,7 @@
       <c r="AK326"/>
       <c r="AL326"/>
     </row>
-    <row r="327" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>409</v>
       </c>
@@ -21280,7 +21296,7 @@
       <c r="AK327"/>
       <c r="AL327"/>
     </row>
-    <row r="328" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>410</v>
       </c>
@@ -21326,7 +21342,7 @@
       <c r="AK328"/>
       <c r="AL328"/>
     </row>
-    <row r="329" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>411</v>
       </c>
@@ -21337,7 +21353,7 @@
         <v>79</v>
       </c>
       <c r="D329" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="E329" t="n">
         <v>4.0</v>
@@ -21390,7 +21406,7 @@
       <c r="AK329"/>
       <c r="AL329"/>
     </row>
-    <row r="330" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>412</v>
       </c>
@@ -21440,7 +21456,7 @@
       <c r="AK330"/>
       <c r="AL330"/>
     </row>
-    <row r="331" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>413</v>
       </c>
@@ -21486,7 +21502,7 @@
       <c r="AK331"/>
       <c r="AL331"/>
     </row>
-    <row r="332" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>414</v>
       </c>
@@ -21536,7 +21552,7 @@
       <c r="AK332"/>
       <c r="AL332"/>
     </row>
-    <row r="333" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>415</v>
       </c>
@@ -21586,7 +21602,7 @@
       <c r="AK333"/>
       <c r="AL333"/>
     </row>
-    <row r="334" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>416</v>
       </c>
@@ -21636,7 +21652,7 @@
       <c r="AK334"/>
       <c r="AL334"/>
     </row>
-    <row r="335" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>417</v>
       </c>
@@ -21688,7 +21704,7 @@
       <c r="AK335"/>
       <c r="AL335"/>
     </row>
-    <row r="336" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>418</v>
       </c>
@@ -21734,7 +21750,7 @@
       <c r="AK336"/>
       <c r="AL336"/>
     </row>
-    <row r="337" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>419</v>
       </c>
@@ -21780,7 +21796,7 @@
       <c r="AK337"/>
       <c r="AL337"/>
     </row>
-    <row r="338" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>420</v>
       </c>
@@ -21830,7 +21846,7 @@
       <c r="AK338"/>
       <c r="AL338"/>
     </row>
-    <row r="339" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>421</v>
       </c>
@@ -21888,7 +21904,7 @@
       <c r="AK339"/>
       <c r="AL339"/>
     </row>
-    <row r="340" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>422</v>
       </c>
@@ -21934,7 +21950,7 @@
       <c r="AK340"/>
       <c r="AL340"/>
     </row>
-    <row r="341" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>423</v>
       </c>
@@ -21984,7 +22000,7 @@
       <c r="AK341"/>
       <c r="AL341"/>
     </row>
-    <row r="342" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>424</v>
       </c>
@@ -22030,7 +22046,7 @@
       <c r="AK342"/>
       <c r="AL342"/>
     </row>
-    <row r="343" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>425</v>
       </c>
@@ -22076,7 +22092,7 @@
       <c r="AK343"/>
       <c r="AL343"/>
     </row>
-    <row r="344" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>426</v>
       </c>
@@ -22122,7 +22138,7 @@
       <c r="AK344"/>
       <c r="AL344"/>
     </row>
-    <row r="345" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>427</v>
       </c>
@@ -22178,7 +22194,7 @@
       <c r="AK345"/>
       <c r="AL345"/>
     </row>
-    <row r="346" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>428</v>
       </c>
@@ -22224,7 +22240,7 @@
       <c r="AK346"/>
       <c r="AL346"/>
     </row>
-    <row r="347" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>429</v>
       </c>
@@ -22270,7 +22286,7 @@
       <c r="AK347"/>
       <c r="AL347"/>
     </row>
-    <row r="348" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>430</v>
       </c>
@@ -22316,7 +22332,7 @@
       <c r="AK348"/>
       <c r="AL348"/>
     </row>
-    <row r="349" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>431</v>
       </c>
@@ -22368,7 +22384,7 @@
       <c r="AK349"/>
       <c r="AL349"/>
     </row>
-    <row r="350" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>432</v>
       </c>
@@ -22414,7 +22430,7 @@
       <c r="AK350"/>
       <c r="AL350"/>
     </row>
-    <row r="351" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>433</v>
       </c>
@@ -22468,7 +22484,7 @@
       <c r="AK351"/>
       <c r="AL351"/>
     </row>
-    <row r="352" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>434</v>
       </c>
@@ -22518,7 +22534,7 @@
       <c r="AK352"/>
       <c r="AL352"/>
     </row>
-    <row r="353" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>435</v>
       </c>
@@ -22578,7 +22594,7 @@
       <c r="AK353"/>
       <c r="AL353"/>
     </row>
-    <row r="354" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>436</v>
       </c>
@@ -22638,7 +22654,7 @@
       <c r="AK354"/>
       <c r="AL354"/>
     </row>
-    <row r="355" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>437</v>
       </c>
@@ -22684,7 +22700,7 @@
       <c r="AK355"/>
       <c r="AL355"/>
     </row>
-    <row r="356" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>438</v>
       </c>
@@ -22730,7 +22746,7 @@
       <c r="AK356"/>
       <c r="AL356"/>
     </row>
-    <row r="357" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>439</v>
       </c>
@@ -22788,7 +22804,7 @@
       <c r="AK357"/>
       <c r="AL357"/>
     </row>
-    <row r="358" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>440</v>
       </c>
@@ -22848,7 +22864,7 @@
       <c r="AK358"/>
       <c r="AL358"/>
     </row>
-    <row r="359" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>441</v>
       </c>
@@ -22908,7 +22924,7 @@
       <c r="AK359"/>
       <c r="AL359"/>
     </row>
-    <row r="360" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>442</v>
       </c>
@@ -22968,7 +22984,7 @@
       <c r="AK360"/>
       <c r="AL360"/>
     </row>
-    <row r="361" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>443</v>
       </c>
@@ -22976,7 +22992,9 @@
         <v>37</v>
       </c>
       <c r="C361"/>
-      <c r="D361"/>
+      <c r="D361" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E361"/>
       <c r="F361"/>
       <c r="G361"/>
@@ -23012,7 +23030,7 @@
       <c r="AK361"/>
       <c r="AL361"/>
     </row>
-    <row r="362" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>444</v>
       </c>
@@ -23070,7 +23088,7 @@
       <c r="AK362"/>
       <c r="AL362"/>
     </row>
-    <row r="363" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>445</v>
       </c>
@@ -23120,7 +23138,7 @@
       <c r="AK363"/>
       <c r="AL363"/>
     </row>
-    <row r="364" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>446</v>
       </c>
@@ -23166,7 +23184,7 @@
       <c r="AK364"/>
       <c r="AL364"/>
     </row>
-    <row r="365" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>447</v>
       </c>
@@ -23212,7 +23230,7 @@
       <c r="AK365"/>
       <c r="AL365"/>
     </row>
-    <row r="366" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>448</v>
       </c>
@@ -23258,7 +23276,7 @@
       <c r="AK366"/>
       <c r="AL366"/>
     </row>
-    <row r="367" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>449</v>
       </c>
@@ -23304,7 +23322,7 @@
       <c r="AK367"/>
       <c r="AL367"/>
     </row>
-    <row r="368" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>450</v>
       </c>
@@ -23362,7 +23380,7 @@
       <c r="AK368"/>
       <c r="AL368"/>
     </row>
-    <row r="369" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>451</v>
       </c>
@@ -23408,7 +23426,7 @@
       <c r="AK369"/>
       <c r="AL369"/>
     </row>
-    <row r="370" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>452</v>
       </c>
@@ -23462,7 +23480,7 @@
       <c r="AK370"/>
       <c r="AL370"/>
     </row>
-    <row r="371" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>453</v>
       </c>
@@ -23508,7 +23526,7 @@
       <c r="AK371"/>
       <c r="AL371"/>
     </row>
-    <row r="372" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>454</v>
       </c>
@@ -23554,7 +23572,7 @@
       <c r="AK372"/>
       <c r="AL372"/>
     </row>
-    <row r="373" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>455</v>
       </c>
@@ -23600,7 +23618,7 @@
       <c r="AK373"/>
       <c r="AL373"/>
     </row>
-    <row r="374" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>456</v>
       </c>
@@ -23650,7 +23668,7 @@
       <c r="AK374"/>
       <c r="AL374"/>
     </row>
-    <row r="375" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>457</v>
       </c>
@@ -23710,7 +23728,7 @@
       <c r="AK375"/>
       <c r="AL375"/>
     </row>
-    <row r="376" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>458</v>
       </c>
@@ -23768,7 +23786,7 @@
       <c r="AK376"/>
       <c r="AL376"/>
     </row>
-    <row r="377" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>459</v>
       </c>
@@ -23828,7 +23846,7 @@
       <c r="AK377"/>
       <c r="AL377"/>
     </row>
-    <row r="378" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>460</v>
       </c>
@@ -23874,7 +23892,7 @@
       <c r="AK378"/>
       <c r="AL378"/>
     </row>
-    <row r="379" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>461</v>
       </c>
@@ -23920,7 +23938,7 @@
       <c r="AK379"/>
       <c r="AL379"/>
     </row>
-    <row r="380" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>462</v>
       </c>
@@ -23966,7 +23984,7 @@
       <c r="AK380"/>
       <c r="AL380"/>
     </row>
-    <row r="381" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>463</v>
       </c>
@@ -24012,7 +24030,7 @@
       <c r="AK381"/>
       <c r="AL381"/>
     </row>
-    <row r="382" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>464</v>
       </c>
@@ -24070,7 +24088,7 @@
       <c r="AK382"/>
       <c r="AL382"/>
     </row>
-    <row r="383" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>465</v>
       </c>
@@ -24116,7 +24134,7 @@
       <c r="AK383"/>
       <c r="AL383"/>
     </row>
-    <row r="384" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>466</v>
       </c>
@@ -24162,7 +24180,7 @@
       <c r="AK384"/>
       <c r="AL384"/>
     </row>
-    <row r="385" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>467</v>
       </c>
@@ -24218,7 +24236,7 @@
       <c r="AK385"/>
       <c r="AL385"/>
     </row>
-    <row r="386" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>468</v>
       </c>
@@ -24264,7 +24282,7 @@
       <c r="AK386"/>
       <c r="AL386"/>
     </row>
-    <row r="387" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>469</v>
       </c>
@@ -24310,7 +24328,7 @@
       <c r="AK387"/>
       <c r="AL387"/>
     </row>
-    <row r="388" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>470</v>
       </c>
@@ -24356,7 +24374,7 @@
       <c r="AK388"/>
       <c r="AL388"/>
     </row>
-    <row r="389" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>471</v>
       </c>
@@ -24402,7 +24420,7 @@
       <c r="AK389"/>
       <c r="AL389"/>
     </row>
-    <row r="390" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>472</v>
       </c>
@@ -24448,7 +24466,7 @@
       <c r="AK390"/>
       <c r="AL390"/>
     </row>
-    <row r="391" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>473</v>
       </c>
@@ -24494,7 +24512,7 @@
       <c r="AK391"/>
       <c r="AL391"/>
     </row>
-    <row r="392" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>474</v>
       </c>
@@ -24552,7 +24570,7 @@
       <c r="AK392"/>
       <c r="AL392"/>
     </row>
-    <row r="393" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>475</v>
       </c>
@@ -24604,7 +24622,7 @@
       <c r="AK393"/>
       <c r="AL393"/>
     </row>
-    <row r="394" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>476</v>
       </c>
@@ -24660,7 +24678,7 @@
       <c r="AK394"/>
       <c r="AL394"/>
     </row>
-    <row r="395" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>477</v>
       </c>
@@ -24712,7 +24730,7 @@
       <c r="AK395"/>
       <c r="AL395"/>
     </row>
-    <row r="396" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>478</v>
       </c>
@@ -24762,7 +24780,7 @@
       <c r="AK396"/>
       <c r="AL396"/>
     </row>
-    <row r="397" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>479</v>
       </c>
@@ -24814,7 +24832,7 @@
       <c r="AK397"/>
       <c r="AL397"/>
     </row>
-    <row r="398" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>480</v>
       </c>
@@ -24870,7 +24888,7 @@
       <c r="AK398"/>
       <c r="AL398"/>
     </row>
-    <row r="399" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>481</v>
       </c>
@@ -24922,7 +24940,7 @@
       <c r="AK399"/>
       <c r="AL399"/>
     </row>
-    <row r="400" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>482</v>
       </c>
@@ -24982,7 +25000,7 @@
       <c r="AK400"/>
       <c r="AL400"/>
     </row>
-    <row r="401" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>483</v>
       </c>
@@ -25030,7 +25048,7 @@
       <c r="AK401"/>
       <c r="AL401"/>
     </row>
-    <row r="402" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>484</v>
       </c>
@@ -25078,7 +25096,7 @@
       <c r="AK402"/>
       <c r="AL402"/>
     </row>
-    <row r="403" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>485</v>
       </c>
@@ -25130,7 +25148,7 @@
       <c r="AK403"/>
       <c r="AL403"/>
     </row>
-    <row r="404" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>486</v>
       </c>
@@ -25182,7 +25200,7 @@
       <c r="AK404"/>
       <c r="AL404"/>
     </row>
-    <row r="405" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>487</v>
       </c>
@@ -25230,7 +25248,7 @@
       <c r="AK405"/>
       <c r="AL405"/>
     </row>
-    <row r="406" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>488</v>
       </c>
@@ -25290,7 +25308,7 @@
       <c r="AK406"/>
       <c r="AL406"/>
     </row>
-    <row r="407" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>489</v>
       </c>
@@ -25348,7 +25366,7 @@
       <c r="AK407"/>
       <c r="AL407"/>
     </row>
-    <row r="408" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>490</v>
       </c>
@@ -25396,7 +25414,7 @@
       <c r="AK408"/>
       <c r="AL408"/>
     </row>
-    <row r="409" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>491</v>
       </c>
@@ -25444,7 +25462,7 @@
       <c r="AK409"/>
       <c r="AL409"/>
     </row>
-    <row r="410" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>492</v>
       </c>
@@ -25492,7 +25510,7 @@
       <c r="AK410"/>
       <c r="AL410"/>
     </row>
-    <row r="411" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>493</v>
       </c>
@@ -25550,7 +25568,7 @@
       <c r="AK411"/>
       <c r="AL411"/>
     </row>
-    <row r="412" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>494</v>
       </c>
@@ -25598,7 +25616,7 @@
       <c r="AK412"/>
       <c r="AL412"/>
     </row>
-    <row r="413" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>495</v>
       </c>
@@ -25646,7 +25664,7 @@
       <c r="AK413"/>
       <c r="AL413"/>
     </row>
-    <row r="414" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>496</v>
       </c>
@@ -25694,7 +25712,7 @@
       <c r="AK414"/>
       <c r="AL414"/>
     </row>
-    <row r="415" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>497</v>
       </c>
@@ -25742,7 +25760,7 @@
       <c r="AK415"/>
       <c r="AL415"/>
     </row>
-    <row r="416" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>498</v>
       </c>
@@ -25790,7 +25808,7 @@
       <c r="AK416"/>
       <c r="AL416"/>
     </row>
-    <row r="417" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>499</v>
       </c>
@@ -25838,7 +25856,7 @@
       <c r="AK417"/>
       <c r="AL417"/>
     </row>
-    <row r="418" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>500</v>
       </c>
@@ -25898,7 +25916,7 @@
       <c r="AK418"/>
       <c r="AL418"/>
     </row>
-    <row r="419" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>501</v>
       </c>
@@ -25946,7 +25964,7 @@
       <c r="AK419"/>
       <c r="AL419"/>
     </row>
-    <row r="420" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>502</v>
       </c>
@@ -26006,7 +26024,7 @@
       <c r="AK420"/>
       <c r="AL420"/>
     </row>
-    <row r="421" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>503</v>
       </c>
@@ -26058,7 +26076,7 @@
       <c r="AK421"/>
       <c r="AL421"/>
     </row>
-    <row r="422" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>504</v>
       </c>
@@ -26114,7 +26132,7 @@
       <c r="AK422"/>
       <c r="AL422"/>
     </row>
-    <row r="423" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>505</v>
       </c>
@@ -26164,7 +26182,7 @@
       <c r="AK423"/>
       <c r="AL423"/>
     </row>
-    <row r="424" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>506</v>
       </c>
@@ -26212,7 +26230,7 @@
       <c r="AK424"/>
       <c r="AL424"/>
     </row>
-    <row r="425" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>507</v>
       </c>
@@ -26264,7 +26282,7 @@
       <c r="AK425"/>
       <c r="AL425"/>
     </row>
-    <row r="426" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>508</v>
       </c>
@@ -26320,7 +26338,7 @@
       <c r="AK426"/>
       <c r="AL426"/>
     </row>
-    <row r="427" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>509</v>
       </c>
@@ -26370,7 +26388,7 @@
       <c r="AK427"/>
       <c r="AL427"/>
     </row>
-    <row r="428" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>510</v>
       </c>
@@ -26381,7 +26399,7 @@
         <v>85</v>
       </c>
       <c r="D428" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E428" t="n">
         <v>5.0</v>
@@ -26430,7 +26448,7 @@
       <c r="AK428"/>
       <c r="AL428"/>
     </row>
-    <row r="429" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>511</v>
       </c>
@@ -26482,7 +26500,7 @@
       <c r="AK429"/>
       <c r="AL429"/>
     </row>
-    <row r="430" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>512</v>
       </c>
@@ -26534,7 +26552,7 @@
       <c r="AK430"/>
       <c r="AL430"/>
     </row>
-    <row r="431" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>513</v>
       </c>
@@ -26598,7 +26616,7 @@
       <c r="AK431"/>
       <c r="AL431"/>
     </row>
-    <row r="432" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>514</v>
       </c>
@@ -26648,7 +26666,7 @@
       <c r="AK432"/>
       <c r="AL432"/>
     </row>
-    <row r="433" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>515</v>
       </c>
@@ -26696,7 +26714,7 @@
       <c r="AK433"/>
       <c r="AL433"/>
     </row>
-    <row r="434" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>516</v>
       </c>
@@ -26746,7 +26764,7 @@
       <c r="AK434"/>
       <c r="AL434"/>
     </row>
-    <row r="435" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>517</v>
       </c>
@@ -26798,7 +26816,7 @@
       <c r="AK435"/>
       <c r="AL435"/>
     </row>
-    <row r="436" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>518</v>
       </c>
@@ -26858,7 +26876,7 @@
       <c r="AK436"/>
       <c r="AL436"/>
     </row>
-    <row r="437" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>519</v>
       </c>
@@ -26912,7 +26930,7 @@
       <c r="AK437"/>
       <c r="AL437"/>
     </row>
-    <row r="438" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>520</v>
       </c>
@@ -26958,7 +26976,7 @@
       <c r="AK438"/>
       <c r="AL438"/>
     </row>
-    <row r="439" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>521</v>
       </c>
@@ -27004,7 +27022,7 @@
       <c r="AK439"/>
       <c r="AL439"/>
     </row>
-    <row r="440" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>522</v>
       </c>
@@ -27054,7 +27072,7 @@
       <c r="AK440"/>
       <c r="AL440"/>
     </row>
-    <row r="441" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>523</v>
       </c>
@@ -27100,7 +27118,7 @@
       <c r="AK441"/>
       <c r="AL441"/>
     </row>
-    <row r="442" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>524</v>
       </c>
@@ -27146,7 +27164,7 @@
       <c r="AK442"/>
       <c r="AL442"/>
     </row>
-    <row r="443" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>525</v>
       </c>
@@ -27192,7 +27210,7 @@
       <c r="AK443"/>
       <c r="AL443"/>
     </row>
-    <row r="444" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>526</v>
       </c>
@@ -27252,7 +27270,7 @@
       <c r="AK444"/>
       <c r="AL444"/>
     </row>
-    <row r="445" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>527</v>
       </c>
@@ -27312,7 +27330,7 @@
       <c r="AK445"/>
       <c r="AL445"/>
     </row>
-    <row r="446" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>528</v>
       </c>
@@ -27374,7 +27392,7 @@
       <c r="AK446"/>
       <c r="AL446"/>
     </row>
-    <row r="447" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>529</v>
       </c>
@@ -27430,7 +27448,7 @@
       <c r="AK447"/>
       <c r="AL447"/>
     </row>
-    <row r="448" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>530</v>
       </c>
@@ -27492,7 +27510,7 @@
       <c r="AK448"/>
       <c r="AL448"/>
     </row>
-    <row r="449" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>531</v>
       </c>
@@ -27542,7 +27560,7 @@
       <c r="AK449"/>
       <c r="AL449"/>
     </row>
-    <row r="450" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>532</v>
       </c>
@@ -27594,7 +27612,7 @@
       <c r="AK450"/>
       <c r="AL450"/>
     </row>
-    <row r="451" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>533</v>
       </c>
@@ -27646,7 +27664,7 @@
       <c r="AK451"/>
       <c r="AL451"/>
     </row>
-    <row r="452" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>534</v>
       </c>
@@ -27696,7 +27714,7 @@
       <c r="AK452"/>
       <c r="AL452"/>
     </row>
-    <row r="453">
+    <row r="453" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>535</v>
       </c>
@@ -27748,7 +27766,7 @@
       <c r="AK453"/>
       <c r="AL453"/>
     </row>
-    <row r="454">
+    <row r="454" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>536</v>
       </c>

</xml_diff>

<commit_message>
Add factory and shipyard to USA
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="4875" windowWidth="37665" windowHeight="13155"/>
+    <workbookView xWindow="15465" yWindow="4875" windowWidth="37665" windowHeight="13155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12996" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="561">
   <si>
     <t>unit</t>
   </si>
@@ -2040,9 +2040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH16" sqref="AH16"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4597,9 +4597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL454"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA42" sqref="AA42"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA437" sqref="AA437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26921,8 +26921,12 @@
       <c r="V438"/>
       <c r="W438"/>
       <c r="X438"/>
-      <c r="Y438"/>
-      <c r="Z438"/>
+      <c r="Y438" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Z438" t="n">
+        <v>1.0</v>
+      </c>
       <c r="AA438"/>
       <c r="AB438"/>
       <c r="AC438"/>

</xml_diff>

<commit_message>
Allow armored trains to certainly defeat enemy trains when attacking. They can only attack if they own the surrounding territory due to canal rules, so the train was trapped behind enemy lines.
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15465" yWindow="4875" windowWidth="37665" windowHeight="13155" activeTab="1"/>
+    <workbookView xWindow="17730" yWindow="4875" windowWidth="37665" windowHeight="13155"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -2040,9 +2040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2287,7 @@
         <v>36</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="L3" t="n">
         <v>2.0</v>
@@ -4597,9 +4597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA437" sqref="AA437"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More starting placement edits
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3660" windowWidth="25760" windowHeight="18840"/>
+    <workbookView xWindow="5520" yWindow="3660" windowWidth="25760" windowHeight="18840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -2060,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
@@ -3416,9 +3416,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ454"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A426" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K448" sqref="K448"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4100,9 +4100,6 @@
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
       <c r="Y25">
         <v>1</v>
       </c>
@@ -6769,11 +6766,11 @@
       <c r="E146">
         <v>4</v>
       </c>
-      <c r="F146">
-        <v>1</v>
-      </c>
       <c r="G146">
         <v>2</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:35" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
First cut at Gas-Munitions
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkavanek/Dropbox/Danny-John Games/GreatWar New Map/TEXT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Danny-John Games\GreatWar New Map\TEXT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3660" windowWidth="25760" windowHeight="18840" activeTab="1"/>
+    <workbookView xWindow="10050" yWindow="3660" windowWidth="25755" windowHeight="18840"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -17,21 +17,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="569">
   <si>
     <t>unit</t>
   </si>
@@ -1732,6 +1729,12 @@
   </si>
   <si>
     <t>Elite-Defensive-InfantryElite-Defensive-Infantry</t>
+  </si>
+  <si>
+    <t>Gas-Munitions</t>
+  </si>
+  <si>
+    <t>1:Gas-Munitions</t>
   </si>
 </sst>
 </file>
@@ -2058,16 +2061,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW40"/>
+  <dimension ref="A1:AW41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="45" max="45" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2274,7 +2280,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2475,7 +2481,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>564</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>565</v>
       </c>
@@ -2579,7 +2585,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>563</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2657,7 +2663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>538</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>562</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>561</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2808,7 +2814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2860,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2933,7 +2939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2955,11 +2961,14 @@
       <c r="L26">
         <v>4</v>
       </c>
+      <c r="Q26" t="s">
+        <v>568</v>
+      </c>
       <c r="AM26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2991,7 +3000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3023,7 +3032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3055,7 +3064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>536</v>
       </c>
@@ -3093,7 +3102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>537</v>
       </c>
@@ -3125,7 +3134,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -3151,7 +3160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -3201,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3233,7 +3242,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -3259,7 +3268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -3323,7 +3332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -3405,6 +3414,32 @@
       </c>
       <c r="X40">
         <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>567</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="AU41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV41" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3416,18 +3451,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H149" sqref="H149"/>
+      <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -3558,7 +3593,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -3572,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -3589,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -3606,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -3623,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3640,7 +3675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -3666,7 +3701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3686,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -3706,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -3723,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -3743,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -3772,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -3804,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -3821,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -3853,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -3870,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -3887,7 +3922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -3913,7 +3948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -3930,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -3959,7 +3994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -3991,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -4020,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -4043,7 +4078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -4072,7 +4107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -4107,7 +4142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -4130,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -4147,7 +4182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -4170,7 +4205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -4193,7 +4228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4216,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4230,7 +4265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4244,7 +4279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4258,7 +4293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -4278,7 +4313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -4304,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -4327,7 +4362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -4344,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -4373,7 +4408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -4399,7 +4434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>559</v>
       </c>
@@ -4410,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -4427,7 +4462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -4459,7 +4494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -4485,7 +4520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -4517,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -4537,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -4554,7 +4589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -4571,7 +4606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>129</v>
       </c>
@@ -4600,7 +4635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -4620,7 +4655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>131</v>
       </c>
@@ -4640,7 +4675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>132</v>
       </c>
@@ -4657,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -4677,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -4694,7 +4729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -4711,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -4725,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -4739,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -4756,7 +4791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -4776,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>141</v>
       </c>
@@ -4787,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>142</v>
       </c>
@@ -4819,7 +4854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -4836,7 +4871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -4853,7 +4888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>145</v>
       </c>
@@ -4882,7 +4917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>146</v>
       </c>
@@ -4911,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -4934,7 +4969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -4960,7 +4995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -4977,7 +5012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>150</v>
       </c>
@@ -4994,7 +5029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>151</v>
       </c>
@@ -5011,7 +5046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>152</v>
       </c>
@@ -5028,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -5060,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>154</v>
       </c>
@@ -5089,7 +5124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>155</v>
       </c>
@@ -5127,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>156</v>
       </c>
@@ -5144,7 +5179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -5161,7 +5196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -5178,7 +5213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -5207,7 +5242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>160</v>
       </c>
@@ -5233,7 +5268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -5253,7 +5288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -5270,7 +5305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -5281,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -5304,7 +5339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -5321,7 +5356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -5338,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>167</v>
       </c>
@@ -5364,7 +5399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -5393,7 +5428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -5410,7 +5445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -5451,7 +5486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -5465,7 +5500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -5485,7 +5520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>173</v>
       </c>
@@ -5499,7 +5534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>174</v>
       </c>
@@ -5516,7 +5551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -5542,7 +5577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -5562,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -5579,7 +5614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -5599,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -5613,7 +5648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -5648,7 +5683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>181</v>
       </c>
@@ -5680,7 +5715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>182</v>
       </c>
@@ -5697,7 +5732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -5723,7 +5758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>184</v>
       </c>
@@ -5743,7 +5778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>185</v>
       </c>
@@ -5784,7 +5819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>186</v>
       </c>
@@ -5810,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>187</v>
       </c>
@@ -5842,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>188</v>
       </c>
@@ -5865,7 +5900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>189</v>
       </c>
@@ -5882,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>190</v>
       </c>
@@ -5917,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>191</v>
       </c>
@@ -5937,7 +5972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>192</v>
       </c>
@@ -5957,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>193</v>
       </c>
@@ -5986,7 +6021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>194</v>
       </c>
@@ -6012,7 +6047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>195</v>
       </c>
@@ -6041,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>196</v>
       </c>
@@ -6076,7 +6111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>197</v>
       </c>
@@ -6093,7 +6128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>198</v>
       </c>
@@ -6110,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>199</v>
       </c>
@@ -6136,7 +6171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>200</v>
       </c>
@@ -6165,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>201</v>
       </c>
@@ -6191,7 +6226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>202</v>
       </c>
@@ -6208,7 +6243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>203</v>
       </c>
@@ -6231,7 +6266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>204</v>
       </c>
@@ -6251,7 +6286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>205</v>
       </c>
@@ -6268,7 +6303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>206</v>
       </c>
@@ -6291,7 +6326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>207</v>
       </c>
@@ -6311,7 +6346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -6322,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>209</v>
       </c>
@@ -6342,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>210</v>
       </c>
@@ -6359,7 +6394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>211</v>
       </c>
@@ -6379,7 +6414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>560</v>
       </c>
@@ -6393,7 +6428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>212</v>
       </c>
@@ -6428,7 +6463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>213</v>
       </c>
@@ -6460,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>214</v>
       </c>
@@ -6474,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>215</v>
       </c>
@@ -6485,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>216</v>
       </c>
@@ -6502,7 +6537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>217</v>
       </c>
@@ -6537,7 +6572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>218</v>
       </c>
@@ -6560,7 +6595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>219</v>
       </c>
@@ -6592,7 +6627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>220</v>
       </c>
@@ -6612,7 +6647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>221</v>
       </c>
@@ -6629,7 +6664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>222</v>
       </c>
@@ -6646,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>223</v>
       </c>
@@ -6678,7 +6713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>224</v>
       </c>
@@ -6707,7 +6742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>225</v>
       </c>
@@ -6727,7 +6762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>226</v>
       </c>
@@ -6750,7 +6785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>227</v>
       </c>
@@ -6773,7 +6808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>228</v>
       </c>
@@ -6787,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>229</v>
       </c>
@@ -6819,7 +6854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>230</v>
       </c>
@@ -6842,7 +6877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>231</v>
       </c>
@@ -6862,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>232</v>
       </c>
@@ -6879,7 +6914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>233</v>
       </c>
@@ -6899,7 +6934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>234</v>
       </c>
@@ -6910,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>235</v>
       </c>
@@ -6921,7 +6956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>236</v>
       </c>
@@ -6932,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>237</v>
       </c>
@@ -6943,7 +6978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>238</v>
       </c>
@@ -6954,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>239</v>
       </c>
@@ -6965,7 +7000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>240</v>
       </c>
@@ -6976,7 +7011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>241</v>
       </c>
@@ -6987,7 +7022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>242</v>
       </c>
@@ -7007,7 +7042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>243</v>
       </c>
@@ -7027,7 +7062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>244</v>
       </c>
@@ -7038,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>245</v>
       </c>
@@ -7049,7 +7084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -7060,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>247</v>
       </c>
@@ -7071,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>248</v>
       </c>
@@ -7082,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>249</v>
       </c>
@@ -7093,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>250</v>
       </c>
@@ -7104,7 +7139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>251</v>
       </c>
@@ -7124,7 +7159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>252</v>
       </c>
@@ -7135,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>253</v>
       </c>
@@ -7155,7 +7190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>254</v>
       </c>
@@ -7175,7 +7210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>255</v>
       </c>
@@ -7189,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>256</v>
       </c>
@@ -7200,7 +7235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>257</v>
       </c>
@@ -7211,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>258</v>
       </c>
@@ -7222,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>259</v>
       </c>
@@ -7233,7 +7268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>260</v>
       </c>
@@ -7244,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>261</v>
       </c>
@@ -7255,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>262</v>
       </c>
@@ -7266,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>263</v>
       </c>
@@ -7277,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>264</v>
       </c>
@@ -7288,7 +7323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>265</v>
       </c>
@@ -7299,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>266</v>
       </c>
@@ -7310,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>267</v>
       </c>
@@ -7321,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>268</v>
       </c>
@@ -7332,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>269</v>
       </c>
@@ -7343,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>270</v>
       </c>
@@ -7354,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>271</v>
       </c>
@@ -7365,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>272</v>
       </c>
@@ -7379,7 +7414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>273</v>
       </c>
@@ -7390,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>274</v>
       </c>
@@ -7401,7 +7436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>275</v>
       </c>
@@ -7412,7 +7447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>276</v>
       </c>
@@ -7423,7 +7458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>277</v>
       </c>
@@ -7443,7 +7478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>278</v>
       </c>
@@ -7454,7 +7489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>279</v>
       </c>
@@ -7465,7 +7500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>280</v>
       </c>
@@ -7476,7 +7511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>281</v>
       </c>
@@ -7487,7 +7522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>282</v>
       </c>
@@ -7498,7 +7533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>283</v>
       </c>
@@ -7509,7 +7544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>284</v>
       </c>
@@ -7520,7 +7555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>285</v>
       </c>
@@ -7531,7 +7566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>286</v>
       </c>
@@ -7542,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>287</v>
       </c>
@@ -7553,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>288</v>
       </c>
@@ -7564,7 +7599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>289</v>
       </c>
@@ -7575,7 +7610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>290</v>
       </c>
@@ -7595,7 +7630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>291</v>
       </c>
@@ -7612,7 +7647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>292</v>
       </c>
@@ -7623,7 +7658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>293</v>
       </c>
@@ -7634,7 +7669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>294</v>
       </c>
@@ -7654,7 +7689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>295</v>
       </c>
@@ -7668,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>296</v>
       </c>
@@ -7679,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>297</v>
       </c>
@@ -7690,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>298</v>
       </c>
@@ -7704,7 +7739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>299</v>
       </c>
@@ -7715,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>300</v>
       </c>
@@ -7726,7 +7761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>301</v>
       </c>
@@ -7743,7 +7778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>302</v>
       </c>
@@ -7754,7 +7789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>303</v>
       </c>
@@ -7771,7 +7806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>304</v>
       </c>
@@ -7782,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>305</v>
       </c>
@@ -7793,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>306</v>
       </c>
@@ -7804,7 +7839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>307</v>
       </c>
@@ -7815,7 +7850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>308</v>
       </c>
@@ -7826,7 +7861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>309</v>
       </c>
@@ -7837,7 +7872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>310</v>
       </c>
@@ -7848,7 +7883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>311</v>
       </c>
@@ -7859,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>312</v>
       </c>
@@ -7879,7 +7914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>313</v>
       </c>
@@ -7890,7 +7925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>314</v>
       </c>
@@ -7901,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>315</v>
       </c>
@@ -7918,7 +7953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>316</v>
       </c>
@@ -7938,7 +7973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>317</v>
       </c>
@@ -7949,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>318</v>
       </c>
@@ -7960,7 +7995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>319</v>
       </c>
@@ -7980,7 +8015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>320</v>
       </c>
@@ -7991,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>321</v>
       </c>
@@ -8002,7 +8037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>322</v>
       </c>
@@ -8013,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>323</v>
       </c>
@@ -8024,7 +8059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>324</v>
       </c>
@@ -8044,7 +8079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>325</v>
       </c>
@@ -8055,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>326</v>
       </c>
@@ -8066,7 +8101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>327</v>
       </c>
@@ -8077,7 +8112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>328</v>
       </c>
@@ -8097,7 +8132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>329</v>
       </c>
@@ -8108,7 +8143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>330</v>
       </c>
@@ -8119,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>331</v>
       </c>
@@ -8130,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>332</v>
       </c>
@@ -8141,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>333</v>
       </c>
@@ -8155,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>334</v>
       </c>
@@ -8166,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>335</v>
       </c>
@@ -8177,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>336</v>
       </c>
@@ -8197,7 +8232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>337</v>
       </c>
@@ -8208,7 +8243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>338</v>
       </c>
@@ -8219,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>339</v>
       </c>
@@ -8233,7 +8268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>340</v>
       </c>
@@ -8244,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>341</v>
       </c>
@@ -8255,7 +8290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>342</v>
       </c>
@@ -8266,7 +8301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>343</v>
       </c>
@@ -8277,7 +8312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>344</v>
       </c>
@@ -8294,7 +8329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>345</v>
       </c>
@@ -8305,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>346</v>
       </c>
@@ -8316,7 +8351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>347</v>
       </c>
@@ -8330,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>348</v>
       </c>
@@ -8341,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>349</v>
       </c>
@@ -8352,7 +8387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>350</v>
       </c>
@@ -8363,7 +8398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>351</v>
       </c>
@@ -8374,7 +8409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>352</v>
       </c>
@@ -8391,7 +8426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>353</v>
       </c>
@@ -8402,7 +8437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>354</v>
       </c>
@@ -8413,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>355</v>
       </c>
@@ -8424,7 +8459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>356</v>
       </c>
@@ -8435,7 +8470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>357</v>
       </c>
@@ -8446,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>358</v>
       </c>
@@ -8457,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>359</v>
       </c>
@@ -8468,7 +8503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>360</v>
       </c>
@@ -8479,7 +8514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>361</v>
       </c>
@@ -8490,7 +8525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>362</v>
       </c>
@@ -8510,7 +8545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>363</v>
       </c>
@@ -8521,7 +8556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>364</v>
       </c>
@@ -8532,7 +8567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>365</v>
       </c>
@@ -8549,7 +8584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>366</v>
       </c>
@@ -8560,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>367</v>
       </c>
@@ -8580,7 +8615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>368</v>
       </c>
@@ -8591,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>369</v>
       </c>
@@ -8602,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>370</v>
       </c>
@@ -8613,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>371</v>
       </c>
@@ -8624,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>372</v>
       </c>
@@ -8635,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>373</v>
       </c>
@@ -8646,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>374</v>
       </c>
@@ -8657,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>375</v>
       </c>
@@ -8668,7 +8703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>376</v>
       </c>
@@ -8679,7 +8714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>377</v>
       </c>
@@ -8690,7 +8725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>378</v>
       </c>
@@ -8701,7 +8736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>379</v>
       </c>
@@ -8712,7 +8747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>380</v>
       </c>
@@ -8723,7 +8758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>381</v>
       </c>
@@ -8746,7 +8781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>382</v>
       </c>
@@ -8769,7 +8804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>383</v>
       </c>
@@ -8801,7 +8836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>384</v>
       </c>
@@ -8818,7 +8853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>385</v>
       </c>
@@ -8832,7 +8867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>386</v>
       </c>
@@ -8855,7 +8890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>387</v>
       </c>
@@ -8869,7 +8904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>388</v>
       </c>
@@ -8886,7 +8921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>389</v>
       </c>
@@ -8909,7 +8944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>390</v>
       </c>
@@ -8935,7 +8970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>391</v>
       </c>
@@ -8973,7 +9008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>392</v>
       </c>
@@ -8996,7 +9031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="312" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>393</v>
       </c>
@@ -9013,7 +9048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>394</v>
       </c>
@@ -9036,7 +9071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>395</v>
       </c>
@@ -9062,7 +9097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>396</v>
       </c>
@@ -9076,7 +9111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>397</v>
       </c>
@@ -9099,7 +9134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>398</v>
       </c>
@@ -9113,7 +9148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>399</v>
       </c>
@@ -9142,7 +9177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>400</v>
       </c>
@@ -9171,7 +9206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>401</v>
       </c>
@@ -9188,7 +9223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>402</v>
       </c>
@@ -9220,7 +9255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>403</v>
       </c>
@@ -9231,7 +9266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>404</v>
       </c>
@@ -9242,7 +9277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>405</v>
       </c>
@@ -9280,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>406</v>
       </c>
@@ -9306,7 +9341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>407</v>
       </c>
@@ -9344,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>408</v>
       </c>
@@ -9355,7 +9390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>409</v>
       </c>
@@ -9366,7 +9401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>410</v>
       </c>
@@ -9404,7 +9439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>411</v>
       </c>
@@ -9421,7 +9456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>412</v>
       </c>
@@ -9432,7 +9467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>413</v>
       </c>
@@ -9449,7 +9484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>414</v>
       </c>
@@ -9466,7 +9501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>415</v>
       </c>
@@ -9483,7 +9518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>416</v>
       </c>
@@ -9503,7 +9538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>417</v>
       </c>
@@ -9514,7 +9549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>418</v>
       </c>
@@ -9525,7 +9560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>419</v>
       </c>
@@ -9542,7 +9577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>420</v>
       </c>
@@ -9577,7 +9612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>421</v>
       </c>
@@ -9588,7 +9623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>422</v>
       </c>
@@ -9605,7 +9640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>423</v>
       </c>
@@ -9616,7 +9651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>424</v>
       </c>
@@ -9627,7 +9662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>425</v>
       </c>
@@ -9638,7 +9673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>426</v>
       </c>
@@ -9664,7 +9699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>427</v>
       </c>
@@ -9675,7 +9710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>428</v>
       </c>
@@ -9686,7 +9721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>429</v>
       </c>
@@ -9697,7 +9732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>430</v>
       </c>
@@ -9717,7 +9752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>431</v>
       </c>
@@ -9728,7 +9763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>432</v>
       </c>
@@ -9757,7 +9792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>433</v>
       </c>
@@ -9774,7 +9809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>434</v>
       </c>
@@ -9806,7 +9841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>435</v>
       </c>
@@ -9838,7 +9873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>436</v>
       </c>
@@ -9849,7 +9884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>437</v>
       </c>
@@ -9860,7 +9895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>438</v>
       </c>
@@ -9889,7 +9924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>439</v>
       </c>
@@ -9921,7 +9956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>440</v>
       </c>
@@ -9953,7 +9988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>441</v>
       </c>
@@ -9985,7 +10020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>442</v>
       </c>
@@ -9996,7 +10031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>443</v>
       </c>
@@ -10025,7 +10060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>444</v>
       </c>
@@ -10042,7 +10077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>445</v>
       </c>
@@ -10053,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>446</v>
       </c>
@@ -10064,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>447</v>
       </c>
@@ -10075,7 +10110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>448</v>
       </c>
@@ -10086,7 +10121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>449</v>
       </c>
@@ -10115,7 +10150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>450</v>
       </c>
@@ -10126,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>451</v>
       </c>
@@ -10149,7 +10184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>452</v>
       </c>
@@ -10160,7 +10195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>453</v>
       </c>
@@ -10171,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>454</v>
       </c>
@@ -10182,7 +10217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>455</v>
       </c>
@@ -10199,7 +10234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>456</v>
       </c>
@@ -10231,7 +10266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>457</v>
       </c>
@@ -10260,7 +10295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>458</v>
       </c>
@@ -10292,7 +10327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>459</v>
       </c>
@@ -10303,7 +10338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>460</v>
       </c>
@@ -10314,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>461</v>
       </c>
@@ -10325,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>462</v>
       </c>
@@ -10336,7 +10371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>463</v>
       </c>
@@ -10365,7 +10400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>464</v>
       </c>
@@ -10376,7 +10411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>465</v>
       </c>
@@ -10387,7 +10422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>466</v>
       </c>
@@ -10416,7 +10451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>467</v>
       </c>
@@ -10427,7 +10462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>468</v>
       </c>
@@ -10438,7 +10473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>469</v>
       </c>
@@ -10449,7 +10484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>470</v>
       </c>
@@ -10460,7 +10495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>471</v>
       </c>
@@ -10471,7 +10506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>472</v>
       </c>
@@ -10482,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>473</v>
       </c>
@@ -10511,7 +10546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>474</v>
       </c>
@@ -10531,7 +10566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>475</v>
       </c>
@@ -10551,7 +10586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>476</v>
       </c>
@@ -10571,7 +10606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>477</v>
       </c>
@@ -10600,7 +10635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>478</v>
       </c>
@@ -10620,7 +10655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>479</v>
       </c>
@@ -10640,7 +10675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>480</v>
       </c>
@@ -10660,7 +10695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>481</v>
       </c>
@@ -10692,7 +10727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>482</v>
       </c>
@@ -10706,7 +10741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>483</v>
       </c>
@@ -10720,7 +10755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>484</v>
       </c>
@@ -10740,7 +10775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>485</v>
       </c>
@@ -10754,7 +10789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>486</v>
       </c>
@@ -10768,7 +10803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>487</v>
       </c>
@@ -10800,7 +10835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>488</v>
       </c>
@@ -10823,7 +10858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>489</v>
       </c>
@@ -10837,7 +10872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>490</v>
       </c>
@@ -10851,7 +10886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>491</v>
       </c>
@@ -10865,7 +10900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>492</v>
       </c>
@@ -10894,7 +10929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>493</v>
       </c>
@@ -10908,7 +10943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>494</v>
       </c>
@@ -10922,7 +10957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>495</v>
       </c>
@@ -10936,7 +10971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>496</v>
       </c>
@@ -10950,7 +10985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>497</v>
       </c>
@@ -10964,7 +10999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>498</v>
       </c>
@@ -10978,7 +11013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>499</v>
       </c>
@@ -10998,7 +11033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>500</v>
       </c>
@@ -11012,7 +11047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>501</v>
       </c>
@@ -11044,7 +11079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="421" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>502</v>
       </c>
@@ -11064,7 +11099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>503</v>
       </c>
@@ -11090,7 +11125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>504</v>
       </c>
@@ -11107,7 +11142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>505</v>
       </c>
@@ -11121,7 +11156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>506</v>
       </c>
@@ -11135,7 +11170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>507</v>
       </c>
@@ -11161,7 +11196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>508</v>
       </c>
@@ -11178,7 +11213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>509</v>
       </c>
@@ -11210,7 +11245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>510</v>
       </c>
@@ -11230,7 +11265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>511</v>
       </c>
@@ -11250,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>512</v>
       </c>
@@ -11288,7 +11323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>513</v>
       </c>
@@ -11305,7 +11340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>514</v>
       </c>
@@ -11319,7 +11354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>515</v>
       </c>
@@ -11336,7 +11371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>516</v>
       </c>
@@ -11356,7 +11391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>517</v>
       </c>
@@ -11388,7 +11423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="437" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>518</v>
       </c>
@@ -11411,7 +11446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>519</v>
       </c>
@@ -11428,7 +11463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>520</v>
       </c>
@@ -11439,7 +11474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>521</v>
       </c>
@@ -11456,7 +11491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>522</v>
       </c>
@@ -11467,7 +11502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>523</v>
       </c>
@@ -11478,7 +11513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>524</v>
       </c>
@@ -11489,7 +11524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>525</v>
       </c>
@@ -11521,7 +11556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>526</v>
       </c>
@@ -11553,7 +11588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>527</v>
       </c>
@@ -11588,7 +11623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>528</v>
       </c>
@@ -11614,7 +11649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>529</v>
       </c>
@@ -11649,7 +11684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>530</v>
       </c>
@@ -11666,7 +11701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>531</v>
       </c>
@@ -11680,7 +11715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>532</v>
       </c>
@@ -11694,7 +11729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>533</v>
       </c>
@@ -11711,7 +11746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>534</v>
       </c>
@@ -11731,7 +11766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>535</v>
       </c>

</xml_diff>

<commit_message>
Update XLSX with latest changes to Gas munitions, bombers, zeppelins, etc.
</commit_message>
<xml_diff>
--- a/over-the-top.xlsx
+++ b/over-the-top.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkavanek/Dropbox/Danny-John Games/GreatWar New Map/TEXT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdimeo\Documents\great-war-1916\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="3660" windowWidth="25760" windowHeight="18840" activeTab="1"/>
+    <workbookView xWindow="12330" yWindow="3660" windowWidth="25755" windowHeight="18840"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -17,21 +17,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="569">
   <si>
     <t>unit</t>
   </si>
@@ -2066,17 +2063,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="45" max="45" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2222,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2254,7 +2251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2283,7 +2280,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2318,7 +2315,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -2356,7 +2353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>37</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -2391,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2423,7 +2420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2452,7 +2449,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2484,7 +2481,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2510,7 +2507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2536,7 +2533,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>564</v>
       </c>
@@ -2562,7 +2559,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>565</v>
       </c>
@@ -2588,7 +2585,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>563</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2640,7 +2637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2666,7 +2663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>538</v>
       </c>
@@ -2692,7 +2689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2718,7 +2715,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>562</v>
       </c>
@@ -2747,7 +2744,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>561</v>
       </c>
@@ -2779,7 +2776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2805,10 +2802,10 @@
         <v>36</v>
       </c>
       <c r="AI21">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AJ21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AK21" t="s">
         <v>36</v>
@@ -2817,7 +2814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2843,7 +2840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2869,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2901,7 +2898,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2942,7 +2939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2971,7 +2968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -3003,7 +3000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3035,7 +3032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>536</v>
       </c>
@@ -3105,7 +3102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>537</v>
       </c>
@@ -3137,7 +3134,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -3163,7 +3160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -3189,10 +3186,10 @@
         <v>36</v>
       </c>
       <c r="AI33">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AJ33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK33" t="s">
         <v>36</v>
@@ -3213,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3245,7 +3242,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -3271,7 +3268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -3300,7 +3297,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -3335,7 +3332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>558</v>
       </c>
@@ -3352,7 +3349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -3384,7 +3381,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -3392,16 +3389,16 @@
         <v>8</v>
       </c>
       <c r="H40">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I40" t="s">
         <v>37</v>
       </c>
       <c r="K40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T40" t="s">
         <v>36</v>
@@ -3419,7 +3416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>567</v>
       </c>
@@ -3433,15 +3430,12 @@
         <v>37</v>
       </c>
       <c r="K41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="AU41" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3454,18 +3448,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L407" sqref="L407"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H380" sqref="H380"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -3596,7 +3590,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -3610,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -3627,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -3644,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -3661,7 +3655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3678,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -3704,7 +3698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3724,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -3744,7 +3738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -3761,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -3781,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -3810,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -3842,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -3859,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -3891,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -3908,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -3925,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -3951,7 +3945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -3968,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -3997,7 +3991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -4029,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -4058,7 +4052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -4081,7 +4075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -4110,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -4145,7 +4139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -4168,7 +4162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -4185,7 +4179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -4208,7 +4202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -4231,7 +4225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4254,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4268,7 +4262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4282,7 +4276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4296,7 +4290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -4316,7 +4310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -4342,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -4365,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -4382,7 +4376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -4411,7 +4405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -4437,7 +4431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>559</v>
       </c>
@@ -4448,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -4465,7 +4459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -4497,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -4523,7 +4517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -4555,7 +4549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -4575,7 +4569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -4592,7 +4586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -4609,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>129</v>
       </c>
@@ -4638,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -4658,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>131</v>
       </c>
@@ -4678,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>132</v>
       </c>
@@ -4695,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -4715,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -4732,7 +4726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -4749,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -4763,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -4777,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -4794,7 +4788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -4814,7 +4808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>141</v>
       </c>
@@ -4825,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>142</v>
       </c>
@@ -4857,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -4874,7 +4868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -4891,7 +4885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>145</v>
       </c>
@@ -4920,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>146</v>
       </c>
@@ -4949,7 +4943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -4972,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -4998,7 +4992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -5015,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>150</v>
       </c>
@@ -5032,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>151</v>
       </c>
@@ -5049,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>152</v>
       </c>
@@ -5066,7 +5060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -5098,7 +5092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>154</v>
       </c>
@@ -5127,7 +5121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>155</v>
       </c>
@@ -5165,7 +5159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>156</v>
       </c>
@@ -5182,7 +5176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -5199,7 +5193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -5216,7 +5210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -5245,7 +5239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>160</v>
       </c>
@@ -5271,7 +5265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -5291,7 +5285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -5308,7 +5302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -5319,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -5342,7 +5336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -5359,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -5376,7 +5370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>167</v>
       </c>
@@ -5402,7 +5396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -5431,7 +5425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -5448,7 +5442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -5489,7 +5483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -5503,7 +5497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -5523,7 +5517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>173</v>
       </c>
@@ -5537,7 +5531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>174</v>
       </c>
@@ -5554,7 +5548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -5580,7 +5574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -5600,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -5617,7 +5611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -5637,7 +5631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -5651,7 +5645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -5686,7 +5680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>181</v>
       </c>
@@ -5718,7 +5712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>182</v>
       </c>
@@ -5735,7 +5729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>183</v>
       </c>
@@ -5761,7 +5755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>184</v>
       </c>
@@ -5781,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>185</v>
       </c>
@@ -5822,7 +5816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>186</v>
       </c>
@@ -5848,7 +5842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>187</v>
       </c>
@@ -5880,7 +5874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>188</v>
       </c>
@@ -5903,7 +5897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>189</v>
       </c>
@@ -5920,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>190</v>
       </c>
@@ -5955,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>191</v>
       </c>
@@ -5975,7 +5969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>192</v>
       </c>
@@ -5995,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>193</v>
       </c>
@@ -6024,7 +6018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>194</v>
       </c>
@@ -6050,7 +6044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>195</v>
       </c>
@@ -6079,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>196</v>
       </c>
@@ -6114,7 +6108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>197</v>
       </c>
@@ -6131,7 +6125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>198</v>
       </c>
@@ -6148,7 +6142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>199</v>
       </c>
@@ -6174,7 +6168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>200</v>
       </c>
@@ -6203,7 +6197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>201</v>
       </c>
@@ -6229,7 +6223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>202</v>
       </c>
@@ -6246,7 +6240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>203</v>
       </c>
@@ -6269,7 +6263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>204</v>
       </c>
@@ -6289,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>205</v>
       </c>
@@ -6306,7 +6300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>206</v>
       </c>
@@ -6329,7 +6323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>207</v>
       </c>
@@ -6349,7 +6343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -6360,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>209</v>
       </c>
@@ -6380,7 +6374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>210</v>
       </c>
@@ -6397,7 +6391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>211</v>
       </c>
@@ -6417,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>560</v>
       </c>
@@ -6431,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>212</v>
       </c>
@@ -6466,7 +6460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>213</v>
       </c>
@@ -6498,7 +6492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>214</v>
       </c>
@@ -6512,7 +6506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>215</v>
       </c>
@@ -6523,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>216</v>
       </c>
@@ -6540,7 +6534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>217</v>
       </c>
@@ -6575,7 +6569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>218</v>
       </c>
@@ -6598,7 +6592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>219</v>
       </c>
@@ -6630,7 +6624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>220</v>
       </c>
@@ -6650,7 +6644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>221</v>
       </c>
@@ -6667,7 +6661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>222</v>
       </c>
@@ -6684,7 +6678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>223</v>
       </c>
@@ -6716,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>224</v>
       </c>
@@ -6745,7 +6739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>225</v>
       </c>
@@ -6765,7 +6759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>226</v>
       </c>
@@ -6788,7 +6782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>227</v>
       </c>
@@ -6811,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>228</v>
       </c>
@@ -6825,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>229</v>
       </c>
@@ -6857,7 +6851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>230</v>
       </c>
@@ -6880,7 +6874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>231</v>
       </c>
@@ -6900,7 +6894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>232</v>
       </c>
@@ -6917,7 +6911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>233</v>
       </c>
@@ -6937,7 +6931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>234</v>
       </c>
@@ -6948,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>235</v>
       </c>
@@ -6959,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>236</v>
       </c>
@@ -6970,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>237</v>
       </c>
@@ -6981,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>238</v>
       </c>
@@ -6992,7 +6986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>239</v>
       </c>
@@ -7003,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>240</v>
       </c>
@@ -7014,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>241</v>
       </c>
@@ -7025,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>242</v>
       </c>
@@ -7045,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>243</v>
       </c>
@@ -7065,7 +7059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>244</v>
       </c>
@@ -7076,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>245</v>
       </c>
@@ -7087,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -7098,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>247</v>
       </c>
@@ -7109,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>248</v>
       </c>
@@ -7120,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>249</v>
       </c>
@@ -7131,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>250</v>
       </c>
@@ -7142,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>251</v>
       </c>
@@ -7162,7 +7156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>252</v>
       </c>
@@ -7173,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>253</v>
       </c>
@@ -7193,7 +7187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>254</v>
       </c>
@@ -7213,7 +7207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>255</v>
       </c>
@@ -7227,7 +7221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>256</v>
       </c>
@@ -7238,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>257</v>
       </c>
@@ -7249,7 +7243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>258</v>
       </c>
@@ -7260,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>259</v>
       </c>
@@ -7271,7 +7265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>260</v>
       </c>
@@ -7282,7 +7276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>261</v>
       </c>
@@ -7293,7 +7287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>262</v>
       </c>
@@ -7304,7 +7298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>263</v>
       </c>
@@ -7315,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>264</v>
       </c>
@@ -7326,7 +7320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>265</v>
       </c>
@@ -7337,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>266</v>
       </c>
@@ -7348,7 +7342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>267</v>
       </c>
@@ -7359,7 +7353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>268</v>
       </c>
@@ -7370,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>269</v>
       </c>
@@ -7381,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>270</v>
       </c>
@@ -7392,7 +7386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>271</v>
       </c>
@@ -7403,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>272</v>
       </c>
@@ -7417,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>273</v>
       </c>
@@ -7428,7 +7422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>274</v>
       </c>
@@ -7439,7 +7433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>275</v>
       </c>
@@ -7450,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>276</v>
       </c>
@@ -7461,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>277</v>
       </c>
@@ -7481,7 +7475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>278</v>
       </c>
@@ -7492,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>279</v>
       </c>
@@ -7503,7 +7497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>280</v>
       </c>
@@ -7514,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>281</v>
       </c>
@@ -7525,7 +7519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>282</v>
       </c>
@@ -7536,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>283</v>
       </c>
@@ -7547,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>284</v>
       </c>
@@ -7558,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>285</v>
       </c>
@@ -7569,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>286</v>
       </c>
@@ -7580,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>287</v>
       </c>
@@ -7591,7 +7585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>288</v>
       </c>
@@ -7602,7 +7596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>289</v>
       </c>
@@ -7613,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>290</v>
       </c>
@@ -7633,7 +7627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>291</v>
       </c>
@@ -7650,7 +7644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>292</v>
       </c>
@@ -7661,7 +7655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>293</v>
       </c>
@@ -7672,7 +7666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>294</v>
       </c>
@@ -7692,7 +7686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>295</v>
       </c>
@@ -7706,7 +7700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>296</v>
       </c>
@@ -7717,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>297</v>
       </c>
@@ -7728,7 +7722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>298</v>
       </c>
@@ -7742,7 +7736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>299</v>
       </c>
@@ -7753,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>300</v>
       </c>
@@ -7764,7 +7758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>301</v>
       </c>
@@ -7781,7 +7775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>302</v>
       </c>
@@ -7792,7 +7786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>303</v>
       </c>
@@ -7809,7 +7803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>304</v>
       </c>
@@ -7820,7 +7814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>305</v>
       </c>
@@ -7831,7 +7825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>306</v>
       </c>
@@ -7842,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>307</v>
       </c>
@@ -7853,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>308</v>
       </c>
@@ -7864,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>309</v>
       </c>
@@ -7875,7 +7869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>310</v>
       </c>
@@ -7886,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>311</v>
       </c>
@@ -7897,7 +7891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>312</v>
       </c>
@@ -7917,7 +7911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>313</v>
       </c>
@@ -7928,7 +7922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>314</v>
       </c>
@@ -7939,7 +7933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>315</v>
       </c>
@@ -7956,7 +7950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>316</v>
       </c>
@@ -7976,7 +7970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>317</v>
       </c>
@@ -7987,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>318</v>
       </c>
@@ -7998,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>319</v>
       </c>
@@ -8018,7 +8012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>320</v>
       </c>
@@ -8029,7 +8023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>321</v>
       </c>
@@ -8040,7 +8034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>322</v>
       </c>
@@ -8051,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>323</v>
       </c>
@@ -8062,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>324</v>
       </c>
@@ -8082,7 +8076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>325</v>
       </c>
@@ -8093,7 +8087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>326</v>
       </c>
@@ -8104,7 +8098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>327</v>
       </c>
@@ -8115,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>328</v>
       </c>
@@ -8135,7 +8129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>329</v>
       </c>
@@ -8146,7 +8140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>330</v>
       </c>
@@ -8157,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>331</v>
       </c>
@@ -8168,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>332</v>
       </c>
@@ -8179,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>333</v>
       </c>
@@ -8193,7 +8187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>334</v>
       </c>
@@ -8204,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>335</v>
       </c>
@@ -8215,7 +8209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>336</v>
       </c>
@@ -8235,7 +8229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>337</v>
       </c>
@@ -8246,7 +8240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>338</v>
       </c>
@@ -8257,7 +8251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>339</v>
       </c>
@@ -8271,7 +8265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>340</v>
       </c>
@@ -8282,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>341</v>
       </c>
@@ -8293,7 +8287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>342</v>
       </c>
@@ -8304,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>343</v>
       </c>
@@ -8315,7 +8309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>344</v>
       </c>
@@ -8332,7 +8326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>345</v>
       </c>
@@ -8343,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>346</v>
       </c>
@@ -8354,7 +8348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>347</v>
       </c>
@@ -8368,7 +8362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>348</v>
       </c>
@@ -8379,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>349</v>
       </c>
@@ -8390,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>350</v>
       </c>
@@ -8401,7 +8395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>351</v>
       </c>
@@ -8412,7 +8406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>352</v>
       </c>
@@ -8429,7 +8423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>353</v>
       </c>
@@ -8440,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>354</v>
       </c>
@@ -8451,7 +8445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>355</v>
       </c>
@@ -8462,7 +8456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>356</v>
       </c>
@@ -8473,7 +8467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>357</v>
       </c>
@@ -8484,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>358</v>
       </c>
@@ -8495,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>359</v>
       </c>
@@ -8506,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>360</v>
       </c>
@@ -8517,7 +8511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>361</v>
       </c>
@@ -8528,7 +8522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>362</v>
       </c>
@@ -8548,7 +8542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>363</v>
       </c>
@@ -8559,7 +8553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>364</v>
       </c>
@@ -8570,7 +8564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>365</v>
       </c>
@@ -8587,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>366</v>
       </c>
@@ -8598,7 +8592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>367</v>
       </c>
@@ -8618,7 +8612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>368</v>
       </c>
@@ -8629,7 +8623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>369</v>
       </c>
@@ -8640,7 +8634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>370</v>
       </c>
@@ -8651,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>371</v>
       </c>
@@ -8662,7 +8656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>372</v>
       </c>
@@ -8673,7 +8667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>373</v>
       </c>
@@ -8684,7 +8678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>374</v>
       </c>
@@ -8695,7 +8689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>375</v>
       </c>
@@ -8706,7 +8700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>376</v>
       </c>
@@ -8717,7 +8711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>377</v>
       </c>
@@ -8728,7 +8722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>378</v>
       </c>
@@ -8739,7 +8733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>379</v>
       </c>
@@ -8750,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>380</v>
       </c>
@@ -8761,7 +8755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>381</v>
       </c>
@@ -8784,7 +8778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>382</v>
       </c>
@@ -8807,7 +8801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>383</v>
       </c>
@@ -8839,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>384</v>
       </c>
@@ -8856,7 +8850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>385</v>
       </c>
@@ -8870,7 +8864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>386</v>
       </c>
@@ -8893,7 +8887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>387</v>
       </c>
@@ -8907,7 +8901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>388</v>
       </c>
@@ -8924,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>389</v>
       </c>
@@ -8947,7 +8941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>390</v>
       </c>
@@ -8973,7 +8967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>391</v>
       </c>
@@ -9011,7 +9005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>392</v>
       </c>
@@ -9034,7 +9028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="312" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>393</v>
       </c>
@@ -9051,7 +9045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>394</v>
       </c>
@@ -9074,7 +9068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>395</v>
       </c>
@@ -9100,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>396</v>
       </c>
@@ -9114,7 +9108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>397</v>
       </c>
@@ -9137,7 +9131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>398</v>
       </c>
@@ -9151,7 +9145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>399</v>
       </c>
@@ -9180,7 +9174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>400</v>
       </c>
@@ -9209,7 +9203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>401</v>
       </c>
@@ -9226,7 +9220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>402</v>
       </c>
@@ -9258,7 +9252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>403</v>
       </c>
@@ -9269,7 +9263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>404</v>
       </c>
@@ -9280,7 +9274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>405</v>
       </c>
@@ -9318,7 +9312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>406</v>
       </c>
@@ -9344,7 +9338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>407</v>
       </c>
@@ -9382,7 +9376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>408</v>
       </c>
@@ -9393,7 +9387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>409</v>
       </c>
@@ -9404,7 +9398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>410</v>
       </c>
@@ -9442,7 +9436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>411</v>
       </c>
@@ -9459,7 +9453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>412</v>
       </c>
@@ -9470,7 +9464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>413</v>
       </c>
@@ -9487,7 +9481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>414</v>
       </c>
@@ -9504,7 +9498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>415</v>
       </c>
@@ -9521,7 +9515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>416</v>
       </c>
@@ -9541,7 +9535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>417</v>
       </c>
@@ -9552,7 +9546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>418</v>
       </c>
@@ -9563,7 +9557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>419</v>
       </c>
@@ -9580,7 +9574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>420</v>
       </c>
@@ -9615,7 +9609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>421</v>
       </c>
@@ -9626,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>422</v>
       </c>
@@ -9643,7 +9637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>423</v>
       </c>
@@ -9654,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>424</v>
       </c>
@@ -9665,7 +9659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>425</v>
       </c>
@@ -9676,7 +9670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>426</v>
       </c>
@@ -9702,7 +9696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>427</v>
       </c>
@@ -9713,7 +9707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>428</v>
       </c>
@@ -9724,7 +9718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>429</v>
       </c>
@@ -9735,7 +9729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>430</v>
       </c>
@@ -9755,7 +9749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>431</v>
       </c>
@@ -9766,7 +9760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>432</v>
       </c>
@@ -9795,7 +9789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>433</v>
       </c>
@@ -9812,7 +9806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>434</v>
       </c>
@@ -9844,7 +9838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>435</v>
       </c>
@@ -9876,7 +9870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>436</v>
       </c>
@@ -9887,7 +9881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>437</v>
       </c>
@@ -9898,7 +9892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>438</v>
       </c>
@@ -9927,7 +9921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>439</v>
       </c>
@@ -9959,7 +9953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>440</v>
       </c>
@@ -9991,7 +9985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>441</v>
       </c>
@@ -10023,7 +10017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>442</v>
       </c>
@@ -10034,7 +10028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>443</v>
       </c>
@@ -10063,7 +10057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>444</v>
       </c>
@@ -10080,7 +10074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>445</v>
       </c>
@@ -10091,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>446</v>
       </c>
@@ -10102,7 +10096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>447</v>
       </c>
@@ -10113,7 +10107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>448</v>
       </c>
@@ -10124,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>449</v>
       </c>
@@ -10153,7 +10147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>450</v>
       </c>
@@ -10164,7 +10158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>451</v>
       </c>
@@ -10187,7 +10181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>452</v>
       </c>
@@ -10198,7 +10192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>453</v>
       </c>
@@ -10209,7 +10203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>454</v>
       </c>
@@ -10220,7 +10214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>455</v>
       </c>
@@ -10237,7 +10231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>456</v>
       </c>
@@ -10269,7 +10263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>457</v>
       </c>
@@ -10298,7 +10292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>458</v>
       </c>
@@ -10330,7 +10324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>459</v>
       </c>
@@ -10341,7 +10335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>460</v>
       </c>
@@ -10352,7 +10346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>461</v>
       </c>
@@ -10363,7 +10357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>462</v>
       </c>
@@ -10374,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>463</v>
       </c>
@@ -10403,7 +10397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>464</v>
       </c>
@@ -10414,7 +10408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>465</v>
       </c>
@@ -10425,7 +10419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>466</v>
       </c>
@@ -10454,7 +10448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>467</v>
       </c>
@@ -10465,7 +10459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>468</v>
       </c>
@@ -10476,7 +10470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>469</v>
       </c>
@@ -10487,7 +10481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>470</v>
       </c>
@@ -10498,7 +10492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>471</v>
       </c>
@@ -10509,7 +10503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>472</v>
       </c>
@@ -10520,7 +10514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>473</v>
       </c>
@@ -10549,7 +10543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>474</v>
       </c>
@@ -10569,7 +10563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>475</v>
       </c>
@@ -10589,7 +10583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>476</v>
       </c>
@@ -10609,7 +10603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>477</v>
       </c>
@@ -10638,7 +10632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>478</v>
       </c>
@@ -10658,7 +10652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>479</v>
       </c>
@@ -10678,7 +10672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>480</v>
       </c>
@@ -10698,7 +10692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>481</v>
       </c>
@@ -10730,7 +10724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>482</v>
       </c>
@@ -10744,7 +10738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>483</v>
       </c>
@@ -10758,7 +10752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>484</v>
       </c>
@@ -10778,7 +10772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>485</v>
       </c>
@@ -10792,7 +10786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>486</v>
       </c>
@@ -10806,7 +10800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>487</v>
       </c>
@@ -10838,7 +10832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>488</v>
       </c>
@@ -10858,7 +10852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>489</v>
       </c>
@@ -10872,7 +10866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>490</v>
       </c>
@@ -10886,7 +10880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>491</v>
       </c>
@@ -10900,7 +10894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>492</v>
       </c>
@@ -10929,7 +10923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>493</v>
       </c>
@@ -10943,7 +10937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>494</v>
       </c>
@@ -10957,7 +10951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>495</v>
       </c>
@@ -10971,7 +10965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>496</v>
       </c>
@@ -10985,7 +10979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>497</v>
       </c>
@@ -10999,7 +10993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>498</v>
       </c>
@@ -11013,7 +11007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>499</v>
       </c>
@@ -11033,7 +11027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>500</v>
       </c>
@@ -11047,7 +11041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>501</v>
       </c>
@@ -11079,7 +11073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="421" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>502</v>
       </c>
@@ -11099,7 +11093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>503</v>
       </c>
@@ -11125,7 +11119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>504</v>
       </c>
@@ -11142,7 +11136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>505</v>
       </c>
@@ -11156,7 +11150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>506</v>
       </c>
@@ -11170,7 +11164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>507</v>
       </c>
@@ -11196,7 +11190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="427" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>508</v>
       </c>
@@ -11213,7 +11207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>509</v>
       </c>
@@ -11245,7 +11239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>510</v>
       </c>
@@ -11265,7 +11259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>511</v>
       </c>
@@ -11285,7 +11279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>512</v>
       </c>
@@ -11323,7 +11317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>513</v>
       </c>
@@ -11340,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>514</v>
       </c>
@@ -11354,7 +11348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>515</v>
       </c>
@@ -11371,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>516</v>
       </c>
@@ -11391,7 +11385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>517</v>
       </c>
@@ -11423,7 +11417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="437" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>518</v>
       </c>
@@ -11446,7 +11440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>519</v>
       </c>
@@ -11463,7 +11457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>520</v>
       </c>
@@ -11474,7 +11468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>521</v>
       </c>
@@ -11491,7 +11485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>522</v>
       </c>
@@ -11502,7 +11496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>523</v>
       </c>
@@ -11513,7 +11507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>524</v>
       </c>
@@ -11524,7 +11518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>525</v>
       </c>
@@ -11556,7 +11550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>526</v>
       </c>
@@ -11588,7 +11582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>527</v>
       </c>
@@ -11623,7 +11617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>528</v>
       </c>
@@ -11649,7 +11643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>529</v>
       </c>
@@ -11684,7 +11678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>530</v>
       </c>
@@ -11701,7 +11695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>531</v>
       </c>
@@ -11715,7 +11709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>532</v>
       </c>
@@ -11729,7 +11723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>533</v>
       </c>
@@ -11746,7 +11740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>534</v>
       </c>
@@ -11766,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>535</v>
       </c>

</xml_diff>